<commit_message>
Imagen konguito soporte cliente
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 6ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 6ª Version.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahdm\Workspace\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6564929A-D988-4310-8BC0-86A354B18685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F270E4-454B-46E2-B01B-5A37D2A84F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="218">
   <si>
     <t>Nombre</t>
   </si>
@@ -695,9 +695,6 @@
     <t>Acabar Bingo</t>
   </si>
   <si>
-    <t>Ventana de juegos de dados</t>
-  </si>
-  <si>
     <t>Conguito de soporte cliente</t>
   </si>
   <si>
@@ -720,6 +717,9 @@
   </si>
   <si>
     <t>Avatares no va</t>
+  </si>
+  <si>
+    <t>Ventana de juegos de dados (Diseñar imagenes)</t>
   </si>
 </sst>
 </file>
@@ -1089,7 +1089,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1173,9 +1173,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1194,7 +1191,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1224,25 +1239,9 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2263,20 +2262,20 @@
   </sheetPr>
   <dimension ref="A2:P177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C177" sqref="C177"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F168" sqref="F168"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="53.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.33203125" customWidth="1"/>
-    <col min="11" max="11" width="35.44140625" customWidth="1"/>
-    <col min="12" max="12" width="26.6640625" customWidth="1"/>
-    <col min="16" max="16" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="5.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" customWidth="1"/>
+    <col min="7" max="7" width="53.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.36328125" customWidth="1"/>
+    <col min="11" max="11" width="35.453125" customWidth="1"/>
+    <col min="12" max="12" width="26.6328125" customWidth="1"/>
+    <col min="16" max="16" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2305,7 +2304,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2314,42 +2313,42 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E996)</f>
-        <v>341.2</v>
+        <v>344.7</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>453.03000000000003</v>
+        <v>453.78000000000003</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="69">
+      <c r="K3" s="74">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73+J130+J145</f>
         <v>121.5</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="60" t="s">
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="69"/>
-    </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="64"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
+      <c r="K4" s="74"/>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="63"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="69"/>
+      <c r="K5" s="74"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
@@ -2369,10 +2368,10 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="70" t="s">
+      <c r="J6" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="66">
+      <c r="K6" s="68">
         <f>F7+F13+F20+F43+F45+F47+F46+J76+J133</f>
         <v>64.5</v>
       </c>
@@ -2395,8 +2394,8 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="66"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="68"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="P7" s="2"/>
@@ -2416,8 +2415,8 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="66"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="68"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="O8" s="2"/>
@@ -2437,10 +2436,10 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="73" t="s">
+      <c r="J9" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="66">
+      <c r="K9" s="68">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+J74+J131+J146</f>
         <v>95.43</v>
       </c>
@@ -2462,8 +2461,8 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="74"/>
-      <c r="K10" s="66"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="68"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
@@ -2480,8 +2479,8 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="66"/>
+      <c r="J11" s="80"/>
+      <c r="K11" s="68"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
@@ -2500,10 +2499,10 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="76" t="s">
+      <c r="J12" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="66">
+      <c r="K12" s="68">
         <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F48+F67+F68+J77+J134+J149</f>
         <v>78.849999999999994</v>
       </c>
@@ -2523,8 +2522,8 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="77"/>
-      <c r="K13" s="66"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="68"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -2541,8 +2540,8 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="66"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="68"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -2559,10 +2558,10 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="79" t="s">
+      <c r="J15" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="66">
+      <c r="K15" s="68">
         <f>F10+F16+F39+F40+F49+F50+F51+J75+J132</f>
         <v>42</v>
       </c>
@@ -2582,8 +2581,8 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="80"/>
-      <c r="K16" s="66"/>
+      <c r="J16" s="70"/>
+      <c r="K16" s="68"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
@@ -2600,8 +2599,8 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="81"/>
-      <c r="K17" s="66"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="68"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
@@ -2620,10 +2619,10 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="67" t="s">
+      <c r="J18" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="66">
+      <c r="K18" s="68">
         <f>F11+F23+F25+F27+F29+F31+F57+F58+F59+F60+F69+F70+J78+J135</f>
         <v>36.75</v>
       </c>
@@ -2646,10 +2645,10 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="68"/>
-      <c r="K19" s="66"/>
-    </row>
-    <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J19" s="73"/>
+      <c r="K19" s="68"/>
+    </row>
+    <row r="20" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
@@ -2666,10 +2665,10 @@
         <v>20</v>
       </c>
       <c r="G20" s="41"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="66"/>
-    </row>
-    <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="J20" s="73"/>
+      <c r="K20" s="68"/>
+    </row>
+    <row r="21" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
@@ -2687,7 +2686,7 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
@@ -2704,13 +2703,13 @@
         <v>5</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="J22" s="59" t="s">
+      <c r="J22" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="59"/>
-      <c r="L22" s="59"/>
-    </row>
-    <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="K22" s="81"/>
+      <c r="L22" s="81"/>
+    </row>
+    <row r="23" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>16</v>
       </c>
@@ -2728,7 +2727,7 @@
       </c>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>13</v>
       </c>
@@ -2746,7 +2745,7 @@
       </c>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>16</v>
       </c>
@@ -2764,7 +2763,7 @@
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>13</v>
       </c>
@@ -2782,7 +2781,7 @@
       </c>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>16</v>
       </c>
@@ -2800,7 +2799,7 @@
       </c>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>13</v>
       </c>
@@ -2818,7 +2817,7 @@
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>16</v>
       </c>
@@ -2836,7 +2835,7 @@
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>13</v>
       </c>
@@ -2854,7 +2853,7 @@
       </c>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>16</v>
       </c>
@@ -2871,7 +2870,7 @@
       <c r="G31" s="7"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>14</v>
       </c>
@@ -2889,7 +2888,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
@@ -2905,7 +2904,7 @@
       </c>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>14</v>
       </c>
@@ -2923,7 +2922,7 @@
       </c>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>14</v>
       </c>
@@ -2941,7 +2940,7 @@
       </c>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
@@ -2959,7 +2958,7 @@
       </c>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>14</v>
       </c>
@@ -2977,7 +2976,7 @@
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>14</v>
       </c>
@@ -2995,7 +2994,7 @@
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>15</v>
       </c>
@@ -3013,7 +3012,7 @@
       </c>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>15</v>
       </c>
@@ -3031,25 +3030,25 @@
       </c>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B41" s="60" t="s">
+    <row r="41" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B41" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="61"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
-    </row>
-    <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B42" s="64"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
-    </row>
-    <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="60"/>
+    </row>
+    <row r="42" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B42" s="63"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="64"/>
+      <c r="F42" s="64"/>
+      <c r="G42" s="64"/>
+    </row>
+    <row r="43" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>12</v>
       </c>
@@ -3067,7 +3066,7 @@
       </c>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>13</v>
       </c>
@@ -3085,7 +3084,7 @@
       </c>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>12</v>
       </c>
@@ -3103,7 +3102,7 @@
       </c>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>12</v>
       </c>
@@ -3121,7 +3120,7 @@
       </c>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>12</v>
       </c>
@@ -3139,7 +3138,7 @@
       </c>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>14</v>
       </c>
@@ -3157,7 +3156,7 @@
       </c>
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B49" s="9" t="s">
         <v>15</v>
       </c>
@@ -3184,7 +3183,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>15</v>
       </c>
@@ -3213,7 +3212,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
         <v>15</v>
       </c>
@@ -3242,7 +3241,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>9</v>
       </c>
@@ -3271,7 +3270,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>9</v>
       </c>
@@ -3300,7 +3299,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>9</v>
       </c>
@@ -3329,7 +3328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
         <v>13</v>
       </c>
@@ -3356,7 +3355,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="56" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
         <v>13</v>
       </c>
@@ -3374,7 +3373,7 @@
       </c>
       <c r="G56" s="11"/>
     </row>
-    <row r="57" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
         <v>16</v>
       </c>
@@ -3392,7 +3391,7 @@
       </c>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
         <v>16</v>
       </c>
@@ -3419,7 +3418,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>16</v>
       </c>
@@ -3448,7 +3447,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="60" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
         <v>16</v>
       </c>
@@ -3477,7 +3476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B61" s="6" t="s">
         <v>13</v>
       </c>
@@ -3719,14 +3718,14 @@
       <c r="G71" s="7"/>
     </row>
     <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="60" t="s">
+      <c r="B72" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="61"/>
-      <c r="D72" s="61"/>
-      <c r="E72" s="61"/>
-      <c r="F72" s="61"/>
-      <c r="G72" s="61"/>
+      <c r="C72" s="60"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="60"/>
+      <c r="F72" s="60"/>
+      <c r="G72" s="60"/>
       <c r="I72" s="33" t="s">
         <v>68</v>
       </c>
@@ -3738,12 +3737,12 @@
       </c>
     </row>
     <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="64"/>
-      <c r="C73" s="65"/>
-      <c r="D73" s="65"/>
-      <c r="E73" s="65"/>
-      <c r="F73" s="65"/>
-      <c r="G73" s="65"/>
+      <c r="B73" s="63"/>
+      <c r="C73" s="64"/>
+      <c r="D73" s="64"/>
+      <c r="E73" s="64"/>
+      <c r="F73" s="64"/>
+      <c r="G73" s="64"/>
       <c r="I73" s="4" t="s">
         <v>9</v>
       </c>
@@ -3995,7 +3994,7 @@
       <c r="F84" s="34"/>
       <c r="G84" s="34"/>
     </row>
-    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B85" s="8" t="s">
         <v>14</v>
       </c>
@@ -4149,7 +4148,7 @@
       </c>
       <c r="G93" s="7"/>
     </row>
-    <row r="94" spans="2:7" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="4" t="s">
         <v>9</v>
       </c>
@@ -4703,22 +4702,22 @@
       <c r="G126" s="50"/>
     </row>
     <row r="127" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="60" t="s">
+      <c r="B127" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="C127" s="61"/>
-      <c r="D127" s="61"/>
-      <c r="E127" s="61"/>
-      <c r="F127" s="61"/>
-      <c r="G127" s="61"/>
+      <c r="C127" s="60"/>
+      <c r="D127" s="60"/>
+      <c r="E127" s="60"/>
+      <c r="F127" s="60"/>
+      <c r="G127" s="60"/>
     </row>
     <row r="128" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="62"/>
-      <c r="C128" s="63"/>
-      <c r="D128" s="63"/>
-      <c r="E128" s="63"/>
-      <c r="F128" s="63"/>
-      <c r="G128" s="63"/>
+      <c r="B128" s="61"/>
+      <c r="C128" s="62"/>
+      <c r="D128" s="62"/>
+      <c r="E128" s="62"/>
+      <c r="F128" s="62"/>
+      <c r="G128" s="62"/>
     </row>
     <row r="129" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="51" t="s">
@@ -5006,22 +5005,22 @@
       <c r="G141" s="7"/>
     </row>
     <row r="142" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="60" t="s">
+      <c r="B142" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="C142" s="61"/>
-      <c r="D142" s="61"/>
-      <c r="E142" s="61"/>
-      <c r="F142" s="61"/>
-      <c r="G142" s="61"/>
+      <c r="C142" s="60"/>
+      <c r="D142" s="60"/>
+      <c r="E142" s="60"/>
+      <c r="F142" s="60"/>
+      <c r="G142" s="60"/>
     </row>
     <row r="143" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="62"/>
-      <c r="C143" s="63"/>
-      <c r="D143" s="63"/>
-      <c r="E143" s="63"/>
-      <c r="F143" s="63"/>
-      <c r="G143" s="63"/>
+      <c r="B143" s="61"/>
+      <c r="C143" s="62"/>
+      <c r="D143" s="62"/>
+      <c r="E143" s="62"/>
+      <c r="F143" s="62"/>
+      <c r="G143" s="62"/>
     </row>
     <row r="144" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="55" t="s">
@@ -5315,22 +5314,22 @@
       <c r="G158" s="7"/>
     </row>
     <row r="159" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="60" t="s">
+      <c r="B159" s="59" t="s">
         <v>201</v>
       </c>
-      <c r="C159" s="61"/>
-      <c r="D159" s="61"/>
-      <c r="E159" s="61"/>
-      <c r="F159" s="61"/>
-      <c r="G159" s="61"/>
+      <c r="C159" s="60"/>
+      <c r="D159" s="60"/>
+      <c r="E159" s="60"/>
+      <c r="F159" s="60"/>
+      <c r="G159" s="60"/>
     </row>
     <row r="160" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B160" s="62"/>
-      <c r="C160" s="63"/>
-      <c r="D160" s="63"/>
-      <c r="E160" s="63"/>
-      <c r="F160" s="63"/>
-      <c r="G160" s="63"/>
+      <c r="B160" s="61"/>
+      <c r="C160" s="62"/>
+      <c r="D160" s="62"/>
+      <c r="E160" s="62"/>
+      <c r="F160" s="62"/>
+      <c r="G160" s="62"/>
       <c r="I160" s="58" t="s">
         <v>188</v>
       </c>
@@ -5351,7 +5350,7 @@
       <c r="D161" s="13"/>
       <c r="E161" s="13"/>
       <c r="F161" s="13"/>
-      <c r="G161" s="82"/>
+      <c r="G161" s="1"/>
       <c r="I161" s="57" t="s">
         <v>9</v>
       </c>
@@ -5366,7 +5365,7 @@
       <c r="D162" s="13"/>
       <c r="E162" s="13"/>
       <c r="F162" s="13"/>
-      <c r="G162" s="82"/>
+      <c r="G162" s="1"/>
       <c r="I162" s="6" t="s">
         <v>13</v>
       </c>
@@ -5381,7 +5380,7 @@
       <c r="D163" s="13"/>
       <c r="E163" s="13"/>
       <c r="F163" s="13"/>
-      <c r="G163" s="82"/>
+      <c r="G163" s="1"/>
       <c r="I163" s="9" t="s">
         <v>15</v>
       </c>
@@ -5396,7 +5395,7 @@
       <c r="D164" s="13"/>
       <c r="E164" s="13"/>
       <c r="F164" s="13"/>
-      <c r="G164" s="82"/>
+      <c r="G164" s="1"/>
       <c r="I164" s="5" t="s">
         <v>12</v>
       </c>
@@ -5411,7 +5410,7 @@
       <c r="D165" s="13"/>
       <c r="E165" s="13"/>
       <c r="F165" s="13"/>
-      <c r="G165" s="82"/>
+      <c r="G165" s="1"/>
       <c r="I165" s="8" t="s">
         <v>14</v>
       </c>
@@ -5426,7 +5425,7 @@
       <c r="D166" s="13"/>
       <c r="E166" s="13"/>
       <c r="F166" s="13"/>
-      <c r="G166" s="82"/>
+      <c r="G166" s="1"/>
       <c r="I166" s="10" t="s">
         <v>16</v>
       </c>
@@ -5441,91 +5440,101 @@
       <c r="D167" s="13"/>
       <c r="E167" s="13"/>
       <c r="F167" s="13"/>
-      <c r="G167" s="82"/>
+      <c r="G167" s="1"/>
     </row>
     <row r="168" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B168" s="54" t="s">
         <v>9</v>
       </c>
       <c r="C168" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="D168" s="13"/>
-      <c r="E168" s="13"/>
+        <v>217</v>
+      </c>
+      <c r="D168" s="13">
+        <v>35</v>
+      </c>
+      <c r="E168" s="13">
+        <v>3</v>
+      </c>
       <c r="F168" s="13"/>
-      <c r="G168" s="82"/>
+      <c r="G168" s="11"/>
     </row>
     <row r="169" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B169" s="54" t="s">
         <v>9</v>
       </c>
       <c r="C169" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="D169" s="13"/>
-      <c r="E169" s="13"/>
-      <c r="F169" s="13"/>
-      <c r="G169" s="82"/>
+        <v>209</v>
+      </c>
+      <c r="D169" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E169" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="F169" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="G169" s="7"/>
     </row>
     <row r="170" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" s="52" t="s">
         <v>13</v>
       </c>
       <c r="C170" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D170" s="13"/>
       <c r="E170" s="13"/>
       <c r="F170" s="13"/>
-      <c r="G170" s="82"/>
+      <c r="G170" s="1"/>
     </row>
     <row r="171" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B171" s="52" t="s">
         <v>13</v>
       </c>
       <c r="C171" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D171" s="13"/>
       <c r="E171" s="13"/>
       <c r="F171" s="13"/>
-      <c r="G171" s="82"/>
+      <c r="G171" s="1"/>
     </row>
     <row r="172" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172" s="52" t="s">
         <v>13</v>
       </c>
       <c r="C172" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D172" s="13"/>
       <c r="E172" s="13"/>
       <c r="F172" s="13"/>
-      <c r="G172" s="82"/>
+      <c r="G172" s="1"/>
     </row>
     <row r="173" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173" s="52" t="s">
         <v>13</v>
       </c>
       <c r="C173" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D173" s="13"/>
       <c r="E173" s="13"/>
       <c r="F173" s="13"/>
-      <c r="G173" s="82"/>
+      <c r="G173" s="1"/>
     </row>
     <row r="174" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B174" s="53" t="s">
         <v>16</v>
       </c>
       <c r="C174" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D174" s="13"/>
       <c r="E174" s="13"/>
       <c r="F174" s="13"/>
-      <c r="G174" s="82"/>
+      <c r="G174" s="1"/>
     </row>
     <row r="175" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175" s="53" t="s">
@@ -5535,34 +5544,36 @@
       <c r="D175" s="13"/>
       <c r="E175" s="13"/>
       <c r="F175" s="13"/>
-      <c r="G175" s="82"/>
+      <c r="G175" s="1"/>
     </row>
     <row r="176" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176" s="51" t="s">
         <v>15</v>
       </c>
       <c r="C176" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D176" s="13"/>
       <c r="E176" s="13"/>
       <c r="F176" s="13"/>
-      <c r="G176" s="82"/>
+      <c r="G176" s="1"/>
     </row>
     <row r="177" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177" s="51" t="s">
         <v>15</v>
       </c>
       <c r="C177" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D177" s="13"/>
       <c r="E177" s="13"/>
       <c r="F177" s="13"/>
-      <c r="G177" s="82"/>
+      <c r="G177" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B72:G73"/>
+    <mergeCell ref="B41:G42"/>
     <mergeCell ref="B159:G160"/>
     <mergeCell ref="B4:G5"/>
     <mergeCell ref="J12:J14"/>
@@ -5579,8 +5590,6 @@
     <mergeCell ref="J22:L22"/>
     <mergeCell ref="B142:G143"/>
     <mergeCell ref="B127:G128"/>
-    <mergeCell ref="B72:G73"/>
-    <mergeCell ref="B41:G42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5600,13 +5609,13 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
+    <col min="3" max="3" width="27.36328125" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5669,7 +5678,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -5692,7 +5701,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -5934,7 +5943,7 @@
       <c r="F17" s="13"/>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -5957,7 +5966,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -5980,7 +5989,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -5994,7 +6003,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -6015,7 +6024,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -6030,7 +6039,7 @@
       <c r="F22" s="13"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -6045,7 +6054,7 @@
       <c r="F23" s="13"/>
       <c r="G23" s="15"/>
     </row>
-    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -6066,7 +6075,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -6081,7 +6090,7 @@
       <c r="F25" s="13"/>
       <c r="G25" s="15"/>
     </row>
-    <row r="26" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -6104,7 +6113,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -6119,7 +6128,7 @@
       <c r="F27" s="13"/>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -6142,7 +6151,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -6157,7 +6166,7 @@
       <c r="F29" s="13"/>
       <c r="G29" s="15"/>
     </row>
-    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -6174,7 +6183,7 @@
       <c r="F30" s="13"/>
       <c r="G30" s="15"/>
     </row>
-    <row r="31" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -6197,7 +6206,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A32" s="15">
         <v>31</v>
       </c>
@@ -6218,7 +6227,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A33" s="15">
         <v>32</v>
       </c>
@@ -6239,7 +6248,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A34" s="15">
         <v>33</v>
       </c>
@@ -6262,7 +6271,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>34</v>
       </c>
@@ -6279,7 +6288,7 @@
       <c r="F35" s="13"/>
       <c r="G35" s="15"/>
     </row>
-    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>35</v>
       </c>
@@ -6294,7 +6303,7 @@
       <c r="F36" s="13"/>
       <c r="G36" s="15"/>
     </row>
-    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>36</v>
       </c>
@@ -6317,7 +6326,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>37</v>
       </c>
@@ -6334,7 +6343,7 @@
       <c r="F38" s="13"/>
       <c r="G38" s="15"/>
     </row>
-    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>38</v>
       </c>
@@ -6349,7 +6358,7 @@
       <c r="F39" s="13"/>
       <c r="G39" s="15"/>
     </row>
-    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>39</v>
       </c>
@@ -6370,7 +6379,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>40</v>
       </c>
@@ -6393,7 +6402,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>41</v>
       </c>
@@ -6416,7 +6425,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>42</v>
       </c>
@@ -6439,7 +6448,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A44" s="15">
         <v>43</v>
       </c>
@@ -6462,7 +6471,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>44</v>
       </c>
@@ -6483,7 +6492,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>45</v>
       </c>
@@ -6500,7 +6509,7 @@
       <c r="F46" s="13"/>
       <c r="G46" s="15"/>
     </row>
-    <row r="47" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>46</v>
       </c>
@@ -6570,23 +6579,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6795,10 +6787,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6821,20 +6841,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
reglas + porcentajes y boton retirarse
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 6ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 6ª Version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE3EB9B-957E-4AA8-8EB1-C9E4EF8D55D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C8CE0D-B160-4108-94A6-EDF8B02750E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="630" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1200,6 +1200,9 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1238,9 +1241,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2263,7 +2263,7 @@
   <dimension ref="A2:P177"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K171" sqref="K171"/>
+      <selection activeCell="E171" sqref="E171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2317,11 +2317,11 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>456.70000000000005</v>
+        <v>460.20000000000005</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="74">
+      <c r="K3" s="75">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73+J130+J145</f>
         <v>121.5</v>
       </c>
@@ -2338,7 +2338,7 @@
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="74"/>
+      <c r="K4" s="75"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="61"/>
@@ -2348,7 +2348,7 @@
       <c r="F5" s="62"/>
       <c r="G5" s="62"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="74"/>
+      <c r="K5" s="75"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
@@ -2368,10 +2368,10 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="75" t="s">
+      <c r="J6" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="68">
+      <c r="K6" s="69">
         <f>F7+F13+F20+F43+F45+F47+F46+J76+J133</f>
         <v>64.5</v>
       </c>
@@ -2394,8 +2394,8 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="68"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="69"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="P7" s="2"/>
@@ -2415,8 +2415,8 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="68"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="69"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="O8" s="2"/>
@@ -2436,10 +2436,10 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="78" t="s">
+      <c r="J9" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="68">
+      <c r="K9" s="69">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+J74+J131+J146</f>
         <v>98.100000000000009</v>
       </c>
@@ -2461,8 +2461,8 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="79"/>
-      <c r="K10" s="68"/>
+      <c r="J10" s="80"/>
+      <c r="K10" s="69"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
@@ -2479,8 +2479,8 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="80"/>
-      <c r="K11" s="68"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="69"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
@@ -2502,7 +2502,7 @@
       <c r="J12" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="68">
+      <c r="K12" s="69">
         <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F48+F67+F68+J77+J134+J149</f>
         <v>78.849999999999994</v>
       </c>
@@ -2523,7 +2523,7 @@
       </c>
       <c r="G13" s="7"/>
       <c r="J13" s="66"/>
-      <c r="K13" s="68"/>
+      <c r="K13" s="69"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="G14" s="7"/>
       <c r="J14" s="67"/>
-      <c r="K14" s="68"/>
+      <c r="K14" s="69"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -2558,10 +2558,10 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="69" t="s">
+      <c r="J15" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="68">
+      <c r="K15" s="69">
         <f>F10+F16+F39+F40+F49+F50+F51+J75+J132</f>
         <v>42</v>
       </c>
@@ -2581,8 +2581,8 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="70"/>
-      <c r="K16" s="68"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="69"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
@@ -2599,8 +2599,8 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="71"/>
-      <c r="K17" s="68"/>
+      <c r="J17" s="72"/>
+      <c r="K17" s="69"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
@@ -2619,10 +2619,10 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="72" t="s">
+      <c r="J18" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="68">
+      <c r="K18" s="69">
         <f>F11+F23+F25+F27+F29+F31+F57+F58+F59+F60+F69+F70+J78+J135</f>
         <v>36.75</v>
       </c>
@@ -2645,8 +2645,8 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="73"/>
-      <c r="K19" s="68"/>
+      <c r="J19" s="74"/>
+      <c r="K19" s="69"/>
     </row>
     <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
@@ -2665,8 +2665,8 @@
         <v>20</v>
       </c>
       <c r="G20" s="41"/>
-      <c r="J20" s="73"/>
-      <c r="K20" s="68"/>
+      <c r="J20" s="74"/>
+      <c r="K20" s="69"/>
     </row>
     <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
@@ -2703,11 +2703,11 @@
         <v>5</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="J22" s="81" t="s">
+      <c r="J22" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="81"/>
-      <c r="L22" s="81"/>
+      <c r="K22" s="68"/>
+      <c r="L22" s="68"/>
     </row>
     <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
@@ -5377,7 +5377,7 @@
       </c>
       <c r="J162">
         <f>F170+F171+F172+F173</f>
-        <v>1</v>
+        <v>4.5</v>
       </c>
       <c r="K162">
         <f>E170+E171+E172+E173</f>
@@ -5494,7 +5494,7 @@
         <v>10</v>
       </c>
       <c r="F170" s="13">
-        <v>1</v>
+        <v>4.5</v>
       </c>
       <c r="G170" s="11"/>
     </row>
@@ -5586,16 +5586,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="K3:K5"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="K6:K8"/>
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="K9:K11"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="K15:K17"/>
-    <mergeCell ref="K18:K20"/>
-    <mergeCell ref="J18:J20"/>
     <mergeCell ref="B72:G73"/>
     <mergeCell ref="B41:G42"/>
     <mergeCell ref="B159:G160"/>
@@ -5604,6 +5596,14 @@
     <mergeCell ref="J22:L22"/>
     <mergeCell ref="B142:G143"/>
     <mergeCell ref="B127:G128"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="K18:K20"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="K3:K5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="K6:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Recoloqué mis cosas del Excel
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 6ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 6ª Version.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7nume\OneDrive\Documentos\CEU\3- Tercero\Software\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8B0007-0ED3-43DA-B2B6-833E9C1F9D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CA98A7-6A34-4173-A502-3349311AE7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="630" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-5445" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -665,9 +665,6 @@
     <t>interfaz de ajustes (continuacion)</t>
   </si>
   <si>
-    <t>Lógica 1 jugador Póker Texas</t>
-  </si>
-  <si>
     <t>Ayuda perfil toolbar</t>
   </si>
   <si>
@@ -723,6 +720,9 @@
   </si>
   <si>
     <t>Diseñar imágenes carta de eleccion</t>
+  </si>
+  <si>
+    <t>Póker Texas</t>
   </si>
 </sst>
 </file>
@@ -1176,34 +1176,22 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1217,6 +1205,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1243,6 +1234,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1311,9 +1311,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>20580</xdr:colOff>
+      <xdr:colOff>16770</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>19568</xdr:rowOff>
+      <xdr:rowOff>15758</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1374,7 +1374,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>16323</xdr:rowOff>
+      <xdr:rowOff>20133</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1433,9 +1433,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>20579</xdr:colOff>
+      <xdr:colOff>16769</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>16230</xdr:rowOff>
+      <xdr:rowOff>20040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1494,9 +1494,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>20579</xdr:colOff>
+      <xdr:colOff>16769</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>15465</xdr:rowOff>
+      <xdr:rowOff>19275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1618,7 +1618,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>19611</xdr:rowOff>
+      <xdr:rowOff>15801</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2263,10 +2263,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:P178"/>
+  <dimension ref="A2:P179"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C182" sqref="C182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2316,42 +2316,42 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E996)</f>
-        <v>359.2</v>
+        <v>360.2</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>464.62000000000006</v>
+        <v>467.12000000000006</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="78">
+      <c r="K3" s="75">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73+J130+J145</f>
         <v>121.5</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="78"/>
+      <c r="K4" s="75"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="65"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="78"/>
+      <c r="K5" s="75"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
@@ -2371,10 +2371,10 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="79" t="s">
+      <c r="J6" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="59">
+      <c r="K6" s="69">
         <f>F7+F13+F20+F43+F45+F47+F46+J76+J133</f>
         <v>64.5</v>
       </c>
@@ -2397,8 +2397,8 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="59"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="69"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="P7" s="2"/>
@@ -2418,8 +2418,8 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="81"/>
-      <c r="K8" s="59"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="69"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="O8" s="2"/>
@@ -2439,10 +2439,10 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="60" t="s">
+      <c r="J9" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="59">
+      <c r="K9" s="69">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+J74+J131+J146+J162</f>
         <v>104.27000000000001</v>
       </c>
@@ -2464,8 +2464,8 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="61"/>
-      <c r="K10" s="59"/>
+      <c r="J10" s="80"/>
+      <c r="K10" s="69"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
@@ -2482,8 +2482,8 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="62"/>
-      <c r="K11" s="59"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="69"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
@@ -2502,10 +2502,10 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="69" t="s">
+      <c r="J12" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="59">
+      <c r="K12" s="69">
         <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F48+F67+F68+J77+J134+J149</f>
         <v>78.849999999999994</v>
       </c>
@@ -2525,8 +2525,8 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="70"/>
-      <c r="K13" s="59"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="69"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -2543,8 +2543,8 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="71"/>
-      <c r="K14" s="59"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="69"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -2561,12 +2561,12 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="73" t="s">
+      <c r="J15" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="59">
-        <f>F10+F16+F39+F40+F49+F50+F51+J75+J132</f>
-        <v>42</v>
+      <c r="K15" s="69">
+        <f>F10+F16+F39+F40+F49+F50+F51+J75+J132+J147+J163</f>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2584,8 +2584,8 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="74"/>
-      <c r="K16" s="59"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="69"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
@@ -2602,8 +2602,8 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="75"/>
-      <c r="K17" s="59"/>
+      <c r="J17" s="72"/>
+      <c r="K17" s="69"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
@@ -2622,10 +2622,10 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="76" t="s">
+      <c r="J18" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="59">
+      <c r="K18" s="69">
         <f>F11+F23+F25+F27+F29+F31+F57+F58+F59+F60+F69+F70+J78+J135</f>
         <v>36.75</v>
       </c>
@@ -2648,8 +2648,8 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="77"/>
-      <c r="K19" s="59"/>
+      <c r="J19" s="74"/>
+      <c r="K19" s="69"/>
     </row>
     <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
@@ -2668,8 +2668,8 @@
         <v>20</v>
       </c>
       <c r="G20" s="41"/>
-      <c r="J20" s="77"/>
-      <c r="K20" s="59"/>
+      <c r="J20" s="74"/>
+      <c r="K20" s="69"/>
     </row>
     <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
@@ -2706,11 +2706,11 @@
         <v>5</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="J22" s="72" t="s">
+      <c r="J22" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="72"/>
-      <c r="L22" s="72"/>
+      <c r="K22" s="68"/>
+      <c r="L22" s="68"/>
     </row>
     <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
@@ -3034,22 +3034,22 @@
       <c r="G40" s="7"/>
     </row>
     <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B41" s="63" t="s">
+      <c r="B41" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="64"/>
-      <c r="D41" s="64"/>
-      <c r="E41" s="64"/>
-      <c r="F41" s="64"/>
-      <c r="G41" s="64"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="60"/>
     </row>
     <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B42" s="65"/>
-      <c r="C42" s="66"/>
-      <c r="D42" s="66"/>
-      <c r="E42" s="66"/>
-      <c r="F42" s="66"/>
-      <c r="G42" s="66"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="64"/>
+      <c r="F42" s="64"/>
+      <c r="G42" s="64"/>
     </row>
     <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
@@ -3721,14 +3721,14 @@
       <c r="G71" s="7"/>
     </row>
     <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="63" t="s">
+      <c r="B72" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="64"/>
-      <c r="D72" s="64"/>
-      <c r="E72" s="64"/>
-      <c r="F72" s="64"/>
-      <c r="G72" s="64"/>
+      <c r="C72" s="60"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="60"/>
+      <c r="F72" s="60"/>
+      <c r="G72" s="60"/>
       <c r="I72" s="33" t="s">
         <v>68</v>
       </c>
@@ -3740,12 +3740,12 @@
       </c>
     </row>
     <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="65"/>
-      <c r="C73" s="66"/>
-      <c r="D73" s="66"/>
-      <c r="E73" s="66"/>
-      <c r="F73" s="66"/>
-      <c r="G73" s="66"/>
+      <c r="B73" s="63"/>
+      <c r="C73" s="64"/>
+      <c r="D73" s="64"/>
+      <c r="E73" s="64"/>
+      <c r="F73" s="64"/>
+      <c r="G73" s="64"/>
       <c r="I73" s="4" t="s">
         <v>9</v>
       </c>
@@ -4705,22 +4705,22 @@
       <c r="G126" s="50"/>
     </row>
     <row r="127" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="63" t="s">
+      <c r="B127" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="C127" s="64"/>
-      <c r="D127" s="64"/>
-      <c r="E127" s="64"/>
-      <c r="F127" s="64"/>
-      <c r="G127" s="64"/>
+      <c r="C127" s="60"/>
+      <c r="D127" s="60"/>
+      <c r="E127" s="60"/>
+      <c r="F127" s="60"/>
+      <c r="G127" s="60"/>
     </row>
     <row r="128" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="67"/>
-      <c r="C128" s="68"/>
-      <c r="D128" s="68"/>
-      <c r="E128" s="68"/>
-      <c r="F128" s="68"/>
-      <c r="G128" s="68"/>
+      <c r="B128" s="61"/>
+      <c r="C128" s="62"/>
+      <c r="D128" s="62"/>
+      <c r="E128" s="62"/>
+      <c r="F128" s="62"/>
+      <c r="G128" s="62"/>
     </row>
     <row r="129" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="51" t="s">
@@ -5008,22 +5008,22 @@
       <c r="G141" s="7"/>
     </row>
     <row r="142" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="63" t="s">
+      <c r="B142" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="C142" s="64"/>
-      <c r="D142" s="64"/>
-      <c r="E142" s="64"/>
-      <c r="F142" s="64"/>
-      <c r="G142" s="64"/>
+      <c r="C142" s="60"/>
+      <c r="D142" s="60"/>
+      <c r="E142" s="60"/>
+      <c r="F142" s="60"/>
+      <c r="G142" s="60"/>
     </row>
     <row r="143" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="67"/>
-      <c r="C143" s="68"/>
-      <c r="D143" s="68"/>
-      <c r="E143" s="68"/>
-      <c r="F143" s="68"/>
-      <c r="G143" s="68"/>
+      <c r="B143" s="61"/>
+      <c r="C143" s="62"/>
+      <c r="D143" s="62"/>
+      <c r="E143" s="62"/>
+      <c r="F143" s="62"/>
+      <c r="G143" s="62"/>
     </row>
     <row r="144" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="55" t="s">
@@ -5118,6 +5118,10 @@
       <c r="I147" s="9" t="s">
         <v>15</v>
       </c>
+      <c r="J147">
+        <f>F155</f>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="148" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" s="52" t="s">
@@ -5276,20 +5280,6 @@
       </c>
       <c r="G155" s="11"/>
     </row>
-    <row r="156" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B156" s="51" t="s">
-        <v>15</v>
-      </c>
-      <c r="C156" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="D156" s="13">
-        <v>15</v>
-      </c>
-      <c r="E156" s="13"/>
-      <c r="F156" s="13"/>
-      <c r="G156" s="11"/>
-    </row>
     <row r="157" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" s="56" t="s">
         <v>14</v>
@@ -5311,7 +5301,7 @@
         <v>14</v>
       </c>
       <c r="C158" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D158" s="13"/>
       <c r="E158" s="13">
@@ -5323,22 +5313,22 @@
       <c r="G158" s="7"/>
     </row>
     <row r="159" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="63" t="s">
-        <v>201</v>
-      </c>
-      <c r="C159" s="64"/>
-      <c r="D159" s="64"/>
-      <c r="E159" s="64"/>
-      <c r="F159" s="64"/>
-      <c r="G159" s="64"/>
+      <c r="B159" s="59" t="s">
+        <v>200</v>
+      </c>
+      <c r="C159" s="60"/>
+      <c r="D159" s="60"/>
+      <c r="E159" s="60"/>
+      <c r="F159" s="60"/>
+      <c r="G159" s="60"/>
     </row>
     <row r="160" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B160" s="67"/>
-      <c r="C160" s="68"/>
-      <c r="D160" s="68"/>
-      <c r="E160" s="68"/>
-      <c r="F160" s="68"/>
-      <c r="G160" s="68"/>
+      <c r="B160" s="61"/>
+      <c r="C160" s="62"/>
+      <c r="D160" s="62"/>
+      <c r="E160" s="62"/>
+      <c r="F160" s="62"/>
+      <c r="G160" s="62"/>
       <c r="I160" s="58" t="s">
         <v>188</v>
       </c>
@@ -5354,7 +5344,7 @@
         <v>14</v>
       </c>
       <c r="C161" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D161" s="13"/>
       <c r="E161" s="13"/>
@@ -5369,7 +5359,7 @@
         <v>14</v>
       </c>
       <c r="C162" s="13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D162" s="13"/>
       <c r="E162" s="13"/>
@@ -5392,7 +5382,7 @@
         <v>14</v>
       </c>
       <c r="C163" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D163" s="13"/>
       <c r="E163" s="13"/>
@@ -5401,13 +5391,21 @@
       <c r="I163" s="9" t="s">
         <v>15</v>
       </c>
+      <c r="J163">
+        <f>F177+F178+F179</f>
+        <v>2.5</v>
+      </c>
+      <c r="K163">
+        <f>E177+E178+E179</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="164" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B164" s="56" t="s">
         <v>14</v>
       </c>
       <c r="C164" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D164" s="13"/>
       <c r="E164" s="13"/>
@@ -5422,7 +5420,7 @@
         <v>12</v>
       </c>
       <c r="C165" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D165" s="13"/>
       <c r="E165" s="13"/>
@@ -5437,7 +5435,7 @@
         <v>12</v>
       </c>
       <c r="C166" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D166" s="13"/>
       <c r="E166" s="13"/>
@@ -5452,7 +5450,7 @@
         <v>9</v>
       </c>
       <c r="C167" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D167" s="13"/>
       <c r="E167" s="13"/>
@@ -5464,7 +5462,7 @@
         <v>9</v>
       </c>
       <c r="C168" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D168" s="13"/>
       <c r="E168" s="13"/>
@@ -5476,7 +5474,7 @@
         <v>9</v>
       </c>
       <c r="C169" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D169" s="13" t="s">
         <v>11</v>
@@ -5494,7 +5492,7 @@
         <v>9</v>
       </c>
       <c r="C170" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D170" s="13">
         <v>35</v>
@@ -5512,7 +5510,7 @@
         <v>13</v>
       </c>
       <c r="C171" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D171" s="15">
         <v>19</v>
@@ -5530,7 +5528,7 @@
         <v>13</v>
       </c>
       <c r="C172" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D172" s="15">
         <v>9</v>
@@ -5544,7 +5542,7 @@
         <v>13</v>
       </c>
       <c r="C173" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D173" s="15">
         <v>39</v>
@@ -5558,7 +5556,7 @@
         <v>13</v>
       </c>
       <c r="C174" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D174" s="13"/>
       <c r="E174" s="13"/>
@@ -5570,7 +5568,7 @@
         <v>16</v>
       </c>
       <c r="C175" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D175" s="13"/>
       <c r="E175" s="13"/>
@@ -5592,11 +5590,17 @@
         <v>15</v>
       </c>
       <c r="C177" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="D177" s="13"/>
-      <c r="E177" s="13"/>
-      <c r="F177" s="13"/>
+        <v>214</v>
+      </c>
+      <c r="D177" s="13">
+        <v>20</v>
+      </c>
+      <c r="E177" s="13">
+        <v>1</v>
+      </c>
+      <c r="F177" s="13">
+        <v>2.5</v>
+      </c>
       <c r="G177" s="1"/>
     </row>
     <row r="178" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5604,15 +5608,31 @@
         <v>15</v>
       </c>
       <c r="C178" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D178" s="13"/>
       <c r="E178" s="13"/>
       <c r="F178" s="13"/>
       <c r="G178" s="1"/>
     </row>
+    <row r="179" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B179" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="C179" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="D179" s="13">
+        <v>15</v>
+      </c>
+      <c r="E179" s="13"/>
+      <c r="F179" s="13"/>
+      <c r="G179" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B72:G73"/>
+    <mergeCell ref="B41:G42"/>
     <mergeCell ref="B159:G160"/>
     <mergeCell ref="B4:G5"/>
     <mergeCell ref="J12:J14"/>
@@ -5629,8 +5649,6 @@
     <mergeCell ref="K6:K8"/>
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="K9:K11"/>
-    <mergeCell ref="B72:G73"/>
-    <mergeCell ref="B41:G42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6620,6 +6638,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6828,38 +6863,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6882,9 +6889,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Excel algo mas -> Gashapon
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 6ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 6ª Version.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E89FC73-7E32-463B-8C11-4E4606E3709B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B01FC0-F2F0-4635-AFED-00196B031A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="218">
   <si>
     <t>Nombre</t>
   </si>
@@ -687,9 +687,6 @@
   </si>
   <si>
     <t>Desafios y Recompensas</t>
-  </si>
-  <si>
-    <t>"algo más"</t>
   </si>
   <si>
     <t>Acabar Bingo</t>
@@ -1176,6 +1173,18 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1206,9 +1215,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1234,15 +1240,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2265,8 +2262,8 @@
   </sheetPr>
   <dimension ref="A2:P178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F171" sqref="F171"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C166" sqref="C166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2324,34 +2321,34 @@
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="75">
+      <c r="K3" s="78">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73+J130+J145</f>
         <v>121.5</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="75"/>
+      <c r="K4" s="78"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="61"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="75"/>
+      <c r="K5" s="78"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
@@ -2371,10 +2368,10 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="76" t="s">
+      <c r="J6" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="69">
+      <c r="K6" s="62">
         <f>F7+F13+F20+F43+F45+F47+F46+J76+J133</f>
         <v>64.5</v>
       </c>
@@ -2397,8 +2394,8 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="69"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="62"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="P7" s="2"/>
@@ -2418,8 +2415,8 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="69"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="62"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="O8" s="2"/>
@@ -2439,10 +2436,10 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="79" t="s">
+      <c r="J9" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="69">
+      <c r="K9" s="62">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+J74+J131+J146+J162</f>
         <v>107.27000000000001</v>
       </c>
@@ -2464,8 +2461,8 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="80"/>
-      <c r="K10" s="69"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="62"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
@@ -2482,8 +2479,8 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="69"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="62"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
@@ -2502,10 +2499,10 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="65" t="s">
+      <c r="J12" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="69">
+      <c r="K12" s="62">
         <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F48+F67+F68+J77+J134+J149</f>
         <v>78.849999999999994</v>
       </c>
@@ -2525,8 +2522,8 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="69"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="62"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -2543,8 +2540,8 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="67"/>
-      <c r="K14" s="69"/>
+      <c r="J14" s="71"/>
+      <c r="K14" s="62"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -2561,10 +2558,10 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="70" t="s">
+      <c r="J15" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="69">
+      <c r="K15" s="62">
         <f>F10+F16+F39+F40+F49+F50+F51+J75+J132</f>
         <v>42</v>
       </c>
@@ -2584,8 +2581,8 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="71"/>
-      <c r="K16" s="69"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="62"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
@@ -2602,8 +2599,8 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="72"/>
-      <c r="K17" s="69"/>
+      <c r="J17" s="75"/>
+      <c r="K17" s="62"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
@@ -2622,10 +2619,10 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="73" t="s">
+      <c r="J18" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="69">
+      <c r="K18" s="62">
         <f>F11+F23+F25+F27+F29+F31+F57+F58+F59+F60+F69+F70+J78+J135</f>
         <v>36.75</v>
       </c>
@@ -2648,8 +2645,8 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="74"/>
-      <c r="K19" s="69"/>
+      <c r="J19" s="77"/>
+      <c r="K19" s="62"/>
     </row>
     <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
@@ -2668,8 +2665,8 @@
         <v>20</v>
       </c>
       <c r="G20" s="41"/>
-      <c r="J20" s="74"/>
-      <c r="K20" s="69"/>
+      <c r="J20" s="77"/>
+      <c r="K20" s="62"/>
     </row>
     <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
@@ -2706,11 +2703,11 @@
         <v>5</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="J22" s="68" t="s">
+      <c r="J22" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="68"/>
-      <c r="L22" s="68"/>
+      <c r="K22" s="72"/>
+      <c r="L22" s="72"/>
     </row>
     <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
@@ -3034,22 +3031,22 @@
       <c r="G40" s="7"/>
     </row>
     <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B41" s="59" t="s">
+      <c r="B41" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="60"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="60"/>
-      <c r="G41" s="60"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="64"/>
+      <c r="E41" s="64"/>
+      <c r="F41" s="64"/>
+      <c r="G41" s="64"/>
     </row>
     <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B42" s="61"/>
-      <c r="C42" s="62"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="62"/>
-      <c r="F42" s="62"/>
-      <c r="G42" s="62"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="66"/>
+      <c r="F42" s="66"/>
+      <c r="G42" s="66"/>
     </row>
     <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
@@ -3721,14 +3718,14 @@
       <c r="G71" s="7"/>
     </row>
     <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="59" t="s">
+      <c r="B72" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="60"/>
-      <c r="D72" s="60"/>
-      <c r="E72" s="60"/>
-      <c r="F72" s="60"/>
-      <c r="G72" s="60"/>
+      <c r="C72" s="64"/>
+      <c r="D72" s="64"/>
+      <c r="E72" s="64"/>
+      <c r="F72" s="64"/>
+      <c r="G72" s="64"/>
       <c r="I72" s="33" t="s">
         <v>68</v>
       </c>
@@ -3740,12 +3737,12 @@
       </c>
     </row>
     <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="61"/>
-      <c r="C73" s="62"/>
-      <c r="D73" s="62"/>
-      <c r="E73" s="62"/>
-      <c r="F73" s="62"/>
-      <c r="G73" s="62"/>
+      <c r="B73" s="65"/>
+      <c r="C73" s="66"/>
+      <c r="D73" s="66"/>
+      <c r="E73" s="66"/>
+      <c r="F73" s="66"/>
+      <c r="G73" s="66"/>
       <c r="I73" s="4" t="s">
         <v>9</v>
       </c>
@@ -4705,22 +4702,22 @@
       <c r="G126" s="50"/>
     </row>
     <row r="127" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="59" t="s">
+      <c r="B127" s="63" t="s">
         <v>176</v>
       </c>
-      <c r="C127" s="60"/>
-      <c r="D127" s="60"/>
-      <c r="E127" s="60"/>
-      <c r="F127" s="60"/>
-      <c r="G127" s="60"/>
+      <c r="C127" s="64"/>
+      <c r="D127" s="64"/>
+      <c r="E127" s="64"/>
+      <c r="F127" s="64"/>
+      <c r="G127" s="64"/>
     </row>
     <row r="128" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="63"/>
-      <c r="C128" s="64"/>
-      <c r="D128" s="64"/>
-      <c r="E128" s="64"/>
-      <c r="F128" s="64"/>
-      <c r="G128" s="64"/>
+      <c r="B128" s="67"/>
+      <c r="C128" s="68"/>
+      <c r="D128" s="68"/>
+      <c r="E128" s="68"/>
+      <c r="F128" s="68"/>
+      <c r="G128" s="68"/>
     </row>
     <row r="129" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="51" t="s">
@@ -5008,22 +5005,22 @@
       <c r="G141" s="7"/>
     </row>
     <row r="142" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="59" t="s">
+      <c r="B142" s="63" t="s">
         <v>187</v>
       </c>
-      <c r="C142" s="60"/>
-      <c r="D142" s="60"/>
-      <c r="E142" s="60"/>
-      <c r="F142" s="60"/>
-      <c r="G142" s="60"/>
+      <c r="C142" s="64"/>
+      <c r="D142" s="64"/>
+      <c r="E142" s="64"/>
+      <c r="F142" s="64"/>
+      <c r="G142" s="64"/>
     </row>
     <row r="143" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="63"/>
-      <c r="C143" s="64"/>
-      <c r="D143" s="64"/>
-      <c r="E143" s="64"/>
-      <c r="F143" s="64"/>
-      <c r="G143" s="64"/>
+      <c r="B143" s="67"/>
+      <c r="C143" s="68"/>
+      <c r="D143" s="68"/>
+      <c r="E143" s="68"/>
+      <c r="F143" s="68"/>
+      <c r="G143" s="68"/>
     </row>
     <row r="144" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="55" t="s">
@@ -5323,22 +5320,22 @@
       <c r="G158" s="7"/>
     </row>
     <row r="159" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="59" t="s">
+      <c r="B159" s="63" t="s">
         <v>201</v>
       </c>
-      <c r="C159" s="60"/>
-      <c r="D159" s="60"/>
-      <c r="E159" s="60"/>
-      <c r="F159" s="60"/>
-      <c r="G159" s="60"/>
+      <c r="C159" s="64"/>
+      <c r="D159" s="64"/>
+      <c r="E159" s="64"/>
+      <c r="F159" s="64"/>
+      <c r="G159" s="64"/>
     </row>
     <row r="160" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B160" s="63"/>
-      <c r="C160" s="64"/>
-      <c r="D160" s="64"/>
-      <c r="E160" s="64"/>
-      <c r="F160" s="64"/>
-      <c r="G160" s="64"/>
+      <c r="B160" s="67"/>
+      <c r="C160" s="68"/>
+      <c r="D160" s="68"/>
+      <c r="E160" s="68"/>
+      <c r="F160" s="68"/>
+      <c r="G160" s="68"/>
       <c r="I160" s="58" t="s">
         <v>188</v>
       </c>
@@ -5437,7 +5434,7 @@
         <v>12</v>
       </c>
       <c r="C166" s="13" t="s">
-        <v>207</v>
+        <v>127</v>
       </c>
       <c r="D166" s="13"/>
       <c r="E166" s="13"/>
@@ -5452,7 +5449,7 @@
         <v>9</v>
       </c>
       <c r="C167" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D167" s="13"/>
       <c r="E167" s="13"/>
@@ -5464,7 +5461,7 @@
         <v>9</v>
       </c>
       <c r="C168" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D168" s="13"/>
       <c r="E168" s="13"/>
@@ -5476,7 +5473,7 @@
         <v>9</v>
       </c>
       <c r="C169" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D169" s="13" t="s">
         <v>11</v>
@@ -5494,7 +5491,7 @@
         <v>9</v>
       </c>
       <c r="C170" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D170" s="13">
         <v>35</v>
@@ -5512,7 +5509,7 @@
         <v>13</v>
       </c>
       <c r="C171" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D171" s="15">
         <v>19</v>
@@ -5530,7 +5527,7 @@
         <v>13</v>
       </c>
       <c r="C172" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D172" s="15">
         <v>9</v>
@@ -5544,7 +5541,7 @@
         <v>13</v>
       </c>
       <c r="C173" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D173" s="15">
         <v>39</v>
@@ -5558,7 +5555,7 @@
         <v>13</v>
       </c>
       <c r="C174" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D174" s="13"/>
       <c r="E174" s="13"/>
@@ -5570,7 +5567,7 @@
         <v>16</v>
       </c>
       <c r="C175" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D175" s="13"/>
       <c r="E175" s="13"/>
@@ -5592,7 +5589,7 @@
         <v>15</v>
       </c>
       <c r="C177" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D177" s="13"/>
       <c r="E177" s="13"/>
@@ -5604,7 +5601,7 @@
         <v>15</v>
       </c>
       <c r="C178" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D178" s="13"/>
       <c r="E178" s="13"/>
@@ -5613,11 +5610,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="B72:G73"/>
-    <mergeCell ref="B41:G42"/>
-    <mergeCell ref="B159:G160"/>
     <mergeCell ref="B4:G5"/>
     <mergeCell ref="J12:J14"/>
     <mergeCell ref="J22:L22"/>
@@ -5631,6 +5623,11 @@
     <mergeCell ref="K3:K5"/>
     <mergeCell ref="J6:J8"/>
     <mergeCell ref="K6:K8"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="B72:G73"/>
+    <mergeCell ref="B41:G42"/>
+    <mergeCell ref="B159:G160"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6620,6 +6617,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6828,38 +6842,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6882,9 +6868,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
cambio de contraseña posible
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 6ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 6ª Version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DC8322-159F-432F-B759-1C43F09BE719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489F9A0A-145F-4556-9A9D-7F86D097FDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1179,6 +1179,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1234,15 +1243,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2265,8 +2265,8 @@
   </sheetPr>
   <dimension ref="A2:P178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F174" sqref="F174"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F172" sqref="F172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2320,38 +2320,38 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>470.96000000000009</v>
+        <v>471.46000000000009</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="75">
+      <c r="K3" s="78">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73+J130+J145</f>
         <v>121.5</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="75"/>
+      <c r="K4" s="78"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="62"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="75"/>
+      <c r="K5" s="78"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
@@ -2371,7 +2371,7 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="76" t="s">
+      <c r="J6" s="79" t="s">
         <v>12</v>
       </c>
       <c r="K6" s="59">
@@ -2397,7 +2397,7 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="77"/>
+      <c r="J7" s="80"/>
       <c r="K7" s="59"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -2418,7 +2418,7 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="78"/>
+      <c r="J8" s="81"/>
       <c r="K8" s="59"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -2439,12 +2439,12 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="79" t="s">
+      <c r="J9" s="60" t="s">
         <v>13</v>
       </c>
       <c r="K9" s="59">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+J74+J131+J146+J162</f>
-        <v>110.61000000000001</v>
+        <v>111.11000000000001</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -2464,7 +2464,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="80"/>
+      <c r="J10" s="61"/>
       <c r="K10" s="59"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2482,7 +2482,7 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="81"/>
+      <c r="J11" s="62"/>
       <c r="K11" s="59"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -2502,7 +2502,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="66" t="s">
+      <c r="J12" s="69" t="s">
         <v>14</v>
       </c>
       <c r="K12" s="59">
@@ -2525,7 +2525,7 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="67"/>
+      <c r="J13" s="70"/>
       <c r="K13" s="59"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2543,7 +2543,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="68"/>
+      <c r="J14" s="71"/>
       <c r="K14" s="59"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2561,7 +2561,7 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="70" t="s">
+      <c r="J15" s="73" t="s">
         <v>15</v>
       </c>
       <c r="K15" s="59">
@@ -2584,7 +2584,7 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="71"/>
+      <c r="J16" s="74"/>
       <c r="K16" s="59"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2602,7 +2602,7 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="72"/>
+      <c r="J17" s="75"/>
       <c r="K17" s="59"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2622,7 +2622,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="73" t="s">
+      <c r="J18" s="76" t="s">
         <v>16</v>
       </c>
       <c r="K18" s="59">
@@ -2648,7 +2648,7 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="74"/>
+      <c r="J19" s="77"/>
       <c r="K19" s="59"/>
     </row>
     <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
@@ -2668,7 +2668,7 @@
         <v>20</v>
       </c>
       <c r="G20" s="41"/>
-      <c r="J20" s="74"/>
+      <c r="J20" s="77"/>
       <c r="K20" s="59"/>
     </row>
     <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
@@ -2706,11 +2706,11 @@
         <v>5</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="J22" s="69" t="s">
+      <c r="J22" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="69"/>
-      <c r="L22" s="69"/>
+      <c r="K22" s="72"/>
+      <c r="L22" s="72"/>
     </row>
     <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
@@ -3034,22 +3034,22 @@
       <c r="G40" s="7"/>
     </row>
     <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B41" s="60" t="s">
+      <c r="B41" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="61"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="64"/>
+      <c r="E41" s="64"/>
+      <c r="F41" s="64"/>
+      <c r="G41" s="64"/>
     </row>
     <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B42" s="62"/>
-      <c r="C42" s="63"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="63"/>
-      <c r="F42" s="63"/>
-      <c r="G42" s="63"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="66"/>
+      <c r="F42" s="66"/>
+      <c r="G42" s="66"/>
     </row>
     <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
@@ -3721,14 +3721,14 @@
       <c r="G71" s="7"/>
     </row>
     <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="60" t="s">
+      <c r="B72" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="61"/>
-      <c r="D72" s="61"/>
-      <c r="E72" s="61"/>
-      <c r="F72" s="61"/>
-      <c r="G72" s="61"/>
+      <c r="C72" s="64"/>
+      <c r="D72" s="64"/>
+      <c r="E72" s="64"/>
+      <c r="F72" s="64"/>
+      <c r="G72" s="64"/>
       <c r="I72" s="33" t="s">
         <v>68</v>
       </c>
@@ -3740,12 +3740,12 @@
       </c>
     </row>
     <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="62"/>
-      <c r="C73" s="63"/>
-      <c r="D73" s="63"/>
-      <c r="E73" s="63"/>
-      <c r="F73" s="63"/>
-      <c r="G73" s="63"/>
+      <c r="B73" s="65"/>
+      <c r="C73" s="66"/>
+      <c r="D73" s="66"/>
+      <c r="E73" s="66"/>
+      <c r="F73" s="66"/>
+      <c r="G73" s="66"/>
       <c r="I73" s="4" t="s">
         <v>9</v>
       </c>
@@ -4705,22 +4705,22 @@
       <c r="G126" s="50"/>
     </row>
     <row r="127" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="60" t="s">
+      <c r="B127" s="63" t="s">
         <v>176</v>
       </c>
-      <c r="C127" s="61"/>
-      <c r="D127" s="61"/>
-      <c r="E127" s="61"/>
-      <c r="F127" s="61"/>
-      <c r="G127" s="61"/>
+      <c r="C127" s="64"/>
+      <c r="D127" s="64"/>
+      <c r="E127" s="64"/>
+      <c r="F127" s="64"/>
+      <c r="G127" s="64"/>
     </row>
     <row r="128" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="64"/>
-      <c r="C128" s="65"/>
-      <c r="D128" s="65"/>
-      <c r="E128" s="65"/>
-      <c r="F128" s="65"/>
-      <c r="G128" s="65"/>
+      <c r="B128" s="67"/>
+      <c r="C128" s="68"/>
+      <c r="D128" s="68"/>
+      <c r="E128" s="68"/>
+      <c r="F128" s="68"/>
+      <c r="G128" s="68"/>
     </row>
     <row r="129" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="51" t="s">
@@ -5008,22 +5008,22 @@
       <c r="G141" s="7"/>
     </row>
     <row r="142" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="60" t="s">
+      <c r="B142" s="63" t="s">
         <v>187</v>
       </c>
-      <c r="C142" s="61"/>
-      <c r="D142" s="61"/>
-      <c r="E142" s="61"/>
-      <c r="F142" s="61"/>
-      <c r="G142" s="61"/>
+      <c r="C142" s="64"/>
+      <c r="D142" s="64"/>
+      <c r="E142" s="64"/>
+      <c r="F142" s="64"/>
+      <c r="G142" s="64"/>
     </row>
     <row r="143" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="64"/>
-      <c r="C143" s="65"/>
-      <c r="D143" s="65"/>
-      <c r="E143" s="65"/>
-      <c r="F143" s="65"/>
-      <c r="G143" s="65"/>
+      <c r="B143" s="67"/>
+      <c r="C143" s="68"/>
+      <c r="D143" s="68"/>
+      <c r="E143" s="68"/>
+      <c r="F143" s="68"/>
+      <c r="G143" s="68"/>
     </row>
     <row r="144" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="55" t="s">
@@ -5323,22 +5323,22 @@
       <c r="G158" s="7"/>
     </row>
     <row r="159" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="60" t="s">
+      <c r="B159" s="63" t="s">
         <v>201</v>
       </c>
-      <c r="C159" s="61"/>
-      <c r="D159" s="61"/>
-      <c r="E159" s="61"/>
-      <c r="F159" s="61"/>
-      <c r="G159" s="61"/>
+      <c r="C159" s="64"/>
+      <c r="D159" s="64"/>
+      <c r="E159" s="64"/>
+      <c r="F159" s="64"/>
+      <c r="G159" s="64"/>
     </row>
     <row r="160" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B160" s="64"/>
-      <c r="C160" s="65"/>
-      <c r="D160" s="65"/>
-      <c r="E160" s="65"/>
-      <c r="F160" s="65"/>
-      <c r="G160" s="65"/>
+      <c r="B160" s="67"/>
+      <c r="C160" s="68"/>
+      <c r="D160" s="68"/>
+      <c r="E160" s="68"/>
+      <c r="F160" s="68"/>
+      <c r="G160" s="68"/>
       <c r="I160" s="58" t="s">
         <v>188</v>
       </c>
@@ -5380,7 +5380,7 @@
       </c>
       <c r="J162">
         <f>F174+F171+F172+F173</f>
-        <v>12.51</v>
+        <v>13.01</v>
       </c>
       <c r="K162">
         <f>E174+E171+E172+E173</f>
@@ -5557,7 +5557,7 @@
         <v>5</v>
       </c>
       <c r="F173" s="13">
-        <v>2.67</v>
+        <v>3.17</v>
       </c>
       <c r="G173" s="11"/>
     </row>
@@ -5625,11 +5625,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="B72:G73"/>
-    <mergeCell ref="B41:G42"/>
     <mergeCell ref="B159:G160"/>
     <mergeCell ref="B4:G5"/>
     <mergeCell ref="J12:J14"/>
@@ -5643,6 +5638,11 @@
     <mergeCell ref="J18:J20"/>
     <mergeCell ref="K3:K5"/>
     <mergeCell ref="J6:J8"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="B72:G73"/>
+    <mergeCell ref="B41:G42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6632,6 +6632,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6840,38 +6857,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6894,9 +6883,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
intentando ganancias otra vez
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 6ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 6ª Version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489F9A0A-145F-4556-9A9D-7F86D097FDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5AFB6D-CB13-461D-8805-A1F54B8759F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1176,34 +1176,22 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1217,6 +1205,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1243,6 +1234,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2266,7 +2266,7 @@
   <dimension ref="A2:P178"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F172" sqref="F172"/>
+      <selection activeCell="F173" sqref="F173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2320,38 +2320,38 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>471.46000000000009</v>
+        <v>472.96000000000009</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="78">
+      <c r="K3" s="75">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73+J130+J145</f>
         <v>121.5</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="78"/>
+      <c r="K4" s="75"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="65"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="78"/>
+      <c r="K5" s="75"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
@@ -2371,10 +2371,10 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="79" t="s">
+      <c r="J6" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="59">
+      <c r="K6" s="69">
         <f>F7+F13+F20+F43+F45+F47+F46+J76+J133</f>
         <v>64.5</v>
       </c>
@@ -2397,8 +2397,8 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="59"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="69"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="P7" s="2"/>
@@ -2418,8 +2418,8 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="81"/>
-      <c r="K8" s="59"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="69"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="O8" s="2"/>
@@ -2439,12 +2439,12 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="60" t="s">
+      <c r="J9" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="59">
+      <c r="K9" s="69">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+J74+J131+J146+J162</f>
-        <v>111.11000000000001</v>
+        <v>112.61000000000001</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -2464,8 +2464,8 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="61"/>
-      <c r="K10" s="59"/>
+      <c r="J10" s="80"/>
+      <c r="K10" s="69"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
@@ -2482,8 +2482,8 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="62"/>
-      <c r="K11" s="59"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="69"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
@@ -2502,10 +2502,10 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="69" t="s">
+      <c r="J12" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="59">
+      <c r="K12" s="69">
         <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F48+F67+F68+J77+J134+J149</f>
         <v>78.849999999999994</v>
       </c>
@@ -2525,8 +2525,8 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="70"/>
-      <c r="K13" s="59"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="69"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -2543,8 +2543,8 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="71"/>
-      <c r="K14" s="59"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="69"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -2561,10 +2561,10 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="73" t="s">
+      <c r="J15" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="59">
+      <c r="K15" s="69">
         <f>F10+F16+F39+F40+F49+F50+F51+J75+J132</f>
         <v>42</v>
       </c>
@@ -2584,8 +2584,8 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="74"/>
-      <c r="K16" s="59"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="69"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
@@ -2602,8 +2602,8 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="75"/>
-      <c r="K17" s="59"/>
+      <c r="J17" s="72"/>
+      <c r="K17" s="69"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
@@ -2622,10 +2622,10 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="76" t="s">
+      <c r="J18" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="59">
+      <c r="K18" s="69">
         <f>F11+F23+F25+F27+F29+F31+F57+F58+F59+F60+F69+F70+J78+J135</f>
         <v>36.75</v>
       </c>
@@ -2648,8 +2648,8 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="77"/>
-      <c r="K19" s="59"/>
+      <c r="J19" s="74"/>
+      <c r="K19" s="69"/>
     </row>
     <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
@@ -2668,8 +2668,8 @@
         <v>20</v>
       </c>
       <c r="G20" s="41"/>
-      <c r="J20" s="77"/>
-      <c r="K20" s="59"/>
+      <c r="J20" s="74"/>
+      <c r="K20" s="69"/>
     </row>
     <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
@@ -2706,11 +2706,11 @@
         <v>5</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="J22" s="72" t="s">
+      <c r="J22" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="72"/>
-      <c r="L22" s="72"/>
+      <c r="K22" s="68"/>
+      <c r="L22" s="68"/>
     </row>
     <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
@@ -3034,22 +3034,22 @@
       <c r="G40" s="7"/>
     </row>
     <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B41" s="63" t="s">
+      <c r="B41" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="64"/>
-      <c r="D41" s="64"/>
-      <c r="E41" s="64"/>
-      <c r="F41" s="64"/>
-      <c r="G41" s="64"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="60"/>
     </row>
     <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B42" s="65"/>
-      <c r="C42" s="66"/>
-      <c r="D42" s="66"/>
-      <c r="E42" s="66"/>
-      <c r="F42" s="66"/>
-      <c r="G42" s="66"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="64"/>
+      <c r="F42" s="64"/>
+      <c r="G42" s="64"/>
     </row>
     <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
@@ -3721,14 +3721,14 @@
       <c r="G71" s="7"/>
     </row>
     <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="63" t="s">
+      <c r="B72" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="64"/>
-      <c r="D72" s="64"/>
-      <c r="E72" s="64"/>
-      <c r="F72" s="64"/>
-      <c r="G72" s="64"/>
+      <c r="C72" s="60"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="60"/>
+      <c r="F72" s="60"/>
+      <c r="G72" s="60"/>
       <c r="I72" s="33" t="s">
         <v>68</v>
       </c>
@@ -3740,12 +3740,12 @@
       </c>
     </row>
     <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="65"/>
-      <c r="C73" s="66"/>
-      <c r="D73" s="66"/>
-      <c r="E73" s="66"/>
-      <c r="F73" s="66"/>
-      <c r="G73" s="66"/>
+      <c r="B73" s="63"/>
+      <c r="C73" s="64"/>
+      <c r="D73" s="64"/>
+      <c r="E73" s="64"/>
+      <c r="F73" s="64"/>
+      <c r="G73" s="64"/>
       <c r="I73" s="4" t="s">
         <v>9</v>
       </c>
@@ -4705,22 +4705,22 @@
       <c r="G126" s="50"/>
     </row>
     <row r="127" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="63" t="s">
+      <c r="B127" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="C127" s="64"/>
-      <c r="D127" s="64"/>
-      <c r="E127" s="64"/>
-      <c r="F127" s="64"/>
-      <c r="G127" s="64"/>
+      <c r="C127" s="60"/>
+      <c r="D127" s="60"/>
+      <c r="E127" s="60"/>
+      <c r="F127" s="60"/>
+      <c r="G127" s="60"/>
     </row>
     <row r="128" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="67"/>
-      <c r="C128" s="68"/>
-      <c r="D128" s="68"/>
-      <c r="E128" s="68"/>
-      <c r="F128" s="68"/>
-      <c r="G128" s="68"/>
+      <c r="B128" s="61"/>
+      <c r="C128" s="62"/>
+      <c r="D128" s="62"/>
+      <c r="E128" s="62"/>
+      <c r="F128" s="62"/>
+      <c r="G128" s="62"/>
     </row>
     <row r="129" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="51" t="s">
@@ -5008,22 +5008,22 @@
       <c r="G141" s="7"/>
     </row>
     <row r="142" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="63" t="s">
+      <c r="B142" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="C142" s="64"/>
-      <c r="D142" s="64"/>
-      <c r="E142" s="64"/>
-      <c r="F142" s="64"/>
-      <c r="G142" s="64"/>
+      <c r="C142" s="60"/>
+      <c r="D142" s="60"/>
+      <c r="E142" s="60"/>
+      <c r="F142" s="60"/>
+      <c r="G142" s="60"/>
     </row>
     <row r="143" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="67"/>
-      <c r="C143" s="68"/>
-      <c r="D143" s="68"/>
-      <c r="E143" s="68"/>
-      <c r="F143" s="68"/>
-      <c r="G143" s="68"/>
+      <c r="B143" s="61"/>
+      <c r="C143" s="62"/>
+      <c r="D143" s="62"/>
+      <c r="E143" s="62"/>
+      <c r="F143" s="62"/>
+      <c r="G143" s="62"/>
     </row>
     <row r="144" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="55" t="s">
@@ -5323,22 +5323,22 @@
       <c r="G158" s="7"/>
     </row>
     <row r="159" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="63" t="s">
+      <c r="B159" s="59" t="s">
         <v>201</v>
       </c>
-      <c r="C159" s="64"/>
-      <c r="D159" s="64"/>
-      <c r="E159" s="64"/>
-      <c r="F159" s="64"/>
-      <c r="G159" s="64"/>
+      <c r="C159" s="60"/>
+      <c r="D159" s="60"/>
+      <c r="E159" s="60"/>
+      <c r="F159" s="60"/>
+      <c r="G159" s="60"/>
     </row>
     <row r="160" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B160" s="67"/>
-      <c r="C160" s="68"/>
-      <c r="D160" s="68"/>
-      <c r="E160" s="68"/>
-      <c r="F160" s="68"/>
-      <c r="G160" s="68"/>
+      <c r="B160" s="61"/>
+      <c r="C160" s="62"/>
+      <c r="D160" s="62"/>
+      <c r="E160" s="62"/>
+      <c r="F160" s="62"/>
+      <c r="G160" s="62"/>
       <c r="I160" s="58" t="s">
         <v>188</v>
       </c>
@@ -5380,7 +5380,7 @@
       </c>
       <c r="J162">
         <f>F174+F171+F172+F173</f>
-        <v>13.01</v>
+        <v>14.51</v>
       </c>
       <c r="K162">
         <f>E174+E171+E172+E173</f>
@@ -5539,7 +5539,7 @@
         <v>2</v>
       </c>
       <c r="F172" s="13">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="G172" s="11"/>
     </row>
@@ -5557,7 +5557,7 @@
         <v>5</v>
       </c>
       <c r="F173" s="13">
-        <v>3.17</v>
+        <v>3.67</v>
       </c>
       <c r="G173" s="11"/>
     </row>
@@ -5625,6 +5625,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B72:G73"/>
+    <mergeCell ref="B41:G42"/>
     <mergeCell ref="B159:G160"/>
     <mergeCell ref="B4:G5"/>
     <mergeCell ref="J12:J14"/>
@@ -5641,8 +5643,6 @@
     <mergeCell ref="K6:K8"/>
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="K9:K11"/>
-    <mergeCell ref="B72:G73"/>
-    <mergeCell ref="B41:G42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6632,23 +6632,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6857,10 +6840,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6883,20 +6894,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Excel de horas ajustadas version 6 si alguien me lo cambia...
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 6ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 6ª Version.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\DaniPC\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1499832-6ECB-42EF-B1FC-1A07E982476A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB782A3-BAC4-43A1-8339-F3B5E150BBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="219">
   <si>
     <t>Nombre</t>
   </si>
@@ -689,9 +689,6 @@
     <t>Desafios y Recompensas</t>
   </si>
   <si>
-    <t>"algo más"</t>
-  </si>
-  <si>
     <t>Acabar Bingo</t>
   </si>
   <si>
@@ -723,6 +720,9 @@
   </si>
   <si>
     <t>Diseñar imágenes carta de eleccion</t>
+  </si>
+  <si>
+    <t>Implementar la plantilla al Tragaperras</t>
   </si>
 </sst>
 </file>
@@ -1176,18 +1176,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1198,12 +1186,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1217,6 +1199,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1243,6 +1234,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2263,10 +2263,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:P178"/>
+  <dimension ref="A2:P179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G170" sqref="G170"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L144" sqref="L144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2316,42 +2316,42 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E996)</f>
-        <v>367.2</v>
+        <v>403.2</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>473.46000000000009</v>
+        <v>490.28000000000009</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="78">
+      <c r="K3" s="75">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73+J130+J145</f>
         <v>121.5</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="78"/>
+      <c r="K4" s="75"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="65"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="78"/>
+      <c r="K5" s="75"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
@@ -2371,12 +2371,12 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="79" t="s">
+      <c r="J6" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="62">
-        <f>F7+F13+F20+F43+F45+F47+F46+J76+J133</f>
-        <v>64.5</v>
+      <c r="K6" s="69">
+        <f>F7+F13+F20+F43+F45+F47+F46+J76+J133+J148+J164</f>
+        <v>91.320000000000007</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -2397,8 +2397,8 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="62"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="69"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="P7" s="2"/>
@@ -2418,8 +2418,8 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="81"/>
-      <c r="K8" s="62"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="69"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="O8" s="2"/>
@@ -2439,10 +2439,10 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="59" t="s">
+      <c r="J9" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="62">
+      <c r="K9" s="69">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+J74+J131+J146+J162</f>
         <v>113.11000000000001</v>
       </c>
@@ -2464,8 +2464,8 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="62"/>
+      <c r="J10" s="80"/>
+      <c r="K10" s="69"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
@@ -2482,8 +2482,8 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="62"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="69"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
@@ -2502,10 +2502,10 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="69" t="s">
+      <c r="J12" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="62">
+      <c r="K12" s="69">
         <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F48+F67+F68+J77+J134+J149</f>
         <v>78.849999999999994</v>
       </c>
@@ -2525,8 +2525,8 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="70"/>
-      <c r="K13" s="62"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="69"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -2543,8 +2543,8 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="71"/>
-      <c r="K14" s="62"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="69"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -2561,10 +2561,10 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="73" t="s">
+      <c r="J15" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="62">
+      <c r="K15" s="69">
         <f>F10+F16+F39+F40+F49+F50+F51+J75+J132</f>
         <v>42</v>
       </c>
@@ -2584,8 +2584,8 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="74"/>
-      <c r="K16" s="62"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="69"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
@@ -2602,8 +2602,8 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="75"/>
-      <c r="K17" s="62"/>
+      <c r="J17" s="72"/>
+      <c r="K17" s="69"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
@@ -2622,10 +2622,10 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="76" t="s">
+      <c r="J18" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="62">
+      <c r="K18" s="69">
         <f>F11+F23+F25+F27+F29+F31+F57+F58+F59+F60+F69+F70+J78+J135</f>
         <v>36.75</v>
       </c>
@@ -2648,8 +2648,8 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="77"/>
-      <c r="K19" s="62"/>
+      <c r="J19" s="74"/>
+      <c r="K19" s="69"/>
     </row>
     <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
@@ -2668,8 +2668,8 @@
         <v>20</v>
       </c>
       <c r="G20" s="41"/>
-      <c r="J20" s="77"/>
-      <c r="K20" s="62"/>
+      <c r="J20" s="74"/>
+      <c r="K20" s="69"/>
     </row>
     <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
@@ -2706,11 +2706,11 @@
         <v>5</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="J22" s="72" t="s">
+      <c r="J22" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="72"/>
-      <c r="L22" s="72"/>
+      <c r="K22" s="66"/>
+      <c r="L22" s="66"/>
     </row>
     <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
@@ -3034,22 +3034,22 @@
       <c r="G40" s="7"/>
     </row>
     <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B41" s="63" t="s">
+      <c r="B41" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="64"/>
-      <c r="D41" s="64"/>
-      <c r="E41" s="64"/>
-      <c r="F41" s="64"/>
-      <c r="G41" s="64"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="60"/>
     </row>
     <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B42" s="65"/>
-      <c r="C42" s="66"/>
-      <c r="D42" s="66"/>
-      <c r="E42" s="66"/>
-      <c r="F42" s="66"/>
-      <c r="G42" s="66"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="62"/>
+      <c r="G42" s="62"/>
     </row>
     <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
@@ -3721,14 +3721,14 @@
       <c r="G71" s="7"/>
     </row>
     <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="63" t="s">
+      <c r="B72" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="64"/>
-      <c r="D72" s="64"/>
-      <c r="E72" s="64"/>
-      <c r="F72" s="64"/>
-      <c r="G72" s="64"/>
+      <c r="C72" s="60"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="60"/>
+      <c r="F72" s="60"/>
+      <c r="G72" s="60"/>
       <c r="I72" s="33" t="s">
         <v>68</v>
       </c>
@@ -3740,12 +3740,12 @@
       </c>
     </row>
     <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="65"/>
-      <c r="C73" s="66"/>
-      <c r="D73" s="66"/>
-      <c r="E73" s="66"/>
-      <c r="F73" s="66"/>
-      <c r="G73" s="66"/>
+      <c r="B73" s="61"/>
+      <c r="C73" s="62"/>
+      <c r="D73" s="62"/>
+      <c r="E73" s="62"/>
+      <c r="F73" s="62"/>
+      <c r="G73" s="62"/>
       <c r="I73" s="4" t="s">
         <v>9</v>
       </c>
@@ -4705,14 +4705,14 @@
       <c r="G126" s="50"/>
     </row>
     <row r="127" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="63" t="s">
+      <c r="B127" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="C127" s="64"/>
-      <c r="D127" s="64"/>
-      <c r="E127" s="64"/>
-      <c r="F127" s="64"/>
-      <c r="G127" s="64"/>
+      <c r="C127" s="60"/>
+      <c r="D127" s="60"/>
+      <c r="E127" s="60"/>
+      <c r="F127" s="60"/>
+      <c r="G127" s="60"/>
     </row>
     <row r="128" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" s="67"/>
@@ -5008,14 +5008,14 @@
       <c r="G141" s="7"/>
     </row>
     <row r="142" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="63" t="s">
+      <c r="B142" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="C142" s="64"/>
-      <c r="D142" s="64"/>
-      <c r="E142" s="64"/>
-      <c r="F142" s="64"/>
-      <c r="G142" s="64"/>
+      <c r="C142" s="60"/>
+      <c r="D142" s="60"/>
+      <c r="E142" s="60"/>
+      <c r="F142" s="60"/>
+      <c r="G142" s="60"/>
     </row>
     <row r="143" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B143" s="67"/>
@@ -5112,8 +5112,12 @@
         <v>192</v>
       </c>
       <c r="D147" s="13"/>
-      <c r="E147" s="13"/>
-      <c r="F147" s="13"/>
+      <c r="E147" s="13">
+        <v>20</v>
+      </c>
+      <c r="F147" s="13">
+        <v>6.34</v>
+      </c>
       <c r="G147" s="11"/>
       <c r="I147" s="9" t="s">
         <v>15</v>
@@ -5141,11 +5145,11 @@
       </c>
       <c r="J148">
         <f>F144+F145+F147</f>
-        <v>10</v>
+        <v>16.34</v>
       </c>
       <c r="K148">
         <f>E144+E145+E147</f>
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="149" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5323,14 +5327,14 @@
       <c r="G158" s="7"/>
     </row>
     <row r="159" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="63" t="s">
+      <c r="B159" s="59" t="s">
         <v>201</v>
       </c>
-      <c r="C159" s="64"/>
-      <c r="D159" s="64"/>
-      <c r="E159" s="64"/>
-      <c r="F159" s="64"/>
-      <c r="G159" s="64"/>
+      <c r="C159" s="60"/>
+      <c r="D159" s="60"/>
+      <c r="E159" s="60"/>
+      <c r="F159" s="60"/>
+      <c r="G159" s="60"/>
     </row>
     <row r="160" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B160" s="67"/>
@@ -5416,6 +5420,14 @@
       <c r="I164" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="J164">
+        <f>F165+F166+F179</f>
+        <v>10.48</v>
+      </c>
+      <c r="K164">
+        <f>E165+E166+E179</f>
+        <v>16</v>
+      </c>
     </row>
     <row r="165" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B165" s="55" t="s">
@@ -5437,11 +5449,15 @@
         <v>12</v>
       </c>
       <c r="C166" s="13" t="s">
-        <v>207</v>
+        <v>127</v>
       </c>
       <c r="D166" s="13"/>
-      <c r="E166" s="13"/>
-      <c r="F166" s="13"/>
+      <c r="E166" s="13">
+        <v>15</v>
+      </c>
+      <c r="F166" s="13">
+        <v>6.48</v>
+      </c>
       <c r="G166" s="1"/>
       <c r="I166" s="10" t="s">
         <v>16</v>
@@ -5452,7 +5468,7 @@
         <v>9</v>
       </c>
       <c r="C167" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D167" s="13"/>
       <c r="E167" s="13"/>
@@ -5464,7 +5480,7 @@
         <v>9</v>
       </c>
       <c r="C168" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D168" s="13"/>
       <c r="E168" s="13"/>
@@ -5476,7 +5492,7 @@
         <v>9</v>
       </c>
       <c r="C169" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D169" s="13" t="s">
         <v>11</v>
@@ -5494,7 +5510,7 @@
         <v>9</v>
       </c>
       <c r="C170" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D170" s="13">
         <v>35</v>
@@ -5512,7 +5528,7 @@
         <v>13</v>
       </c>
       <c r="C171" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D171" s="15">
         <v>19</v>
@@ -5530,7 +5546,7 @@
         <v>13</v>
       </c>
       <c r="C172" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D172" s="15">
         <v>9</v>
@@ -5548,7 +5564,7 @@
         <v>13</v>
       </c>
       <c r="C173" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D173" s="15">
         <v>39</v>
@@ -5566,7 +5582,7 @@
         <v>13</v>
       </c>
       <c r="C174" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D174" s="13"/>
       <c r="E174" s="13">
@@ -5582,7 +5598,7 @@
         <v>16</v>
       </c>
       <c r="C175" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D175" s="13"/>
       <c r="E175" s="13"/>
@@ -5604,7 +5620,7 @@
         <v>15</v>
       </c>
       <c r="C177" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D177" s="13"/>
       <c r="E177" s="13"/>
@@ -5616,15 +5632,33 @@
         <v>15</v>
       </c>
       <c r="C178" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D178" s="13"/>
       <c r="E178" s="13"/>
       <c r="F178" s="13"/>
       <c r="G178" s="1"/>
     </row>
+    <row r="179" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B179" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="C179" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="D179" s="13"/>
+      <c r="E179" s="13">
+        <v>1</v>
+      </c>
+      <c r="F179" s="13">
+        <v>4</v>
+      </c>
+      <c r="G179" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B41:G42"/>
+    <mergeCell ref="B159:G160"/>
     <mergeCell ref="B4:G5"/>
     <mergeCell ref="J12:J14"/>
     <mergeCell ref="J22:L22"/>
@@ -5641,8 +5675,6 @@
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="K9:K11"/>
     <mergeCell ref="B72:G73"/>
-    <mergeCell ref="B41:G42"/>
-    <mergeCell ref="B159:G160"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6632,6 +6664,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6840,38 +6889,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6894,9 +6915,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Excel y arreglado ruleta rusa merengue merengue
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 6ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 6ª Version.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanzc\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\DaniPC\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD5AD9F-3B6B-4F46-B79C-7506A28F3B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745939AE-14B8-4E19-A545-A79B3E6007B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="220">
   <si>
     <t>Nombre</t>
   </si>
@@ -723,6 +723,9 @@
   </si>
   <si>
     <t>Implementar la plantilla al Tragaperras</t>
+  </si>
+  <si>
+    <t>Solucionando errores (tragaperras, blackjack y ruleta rusa)</t>
   </si>
 </sst>
 </file>
@@ -732,7 +735,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -806,6 +809,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="23">
@@ -1092,7 +1102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1176,6 +1186,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1205,9 +1218,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1245,6 +1255,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2263,25 +2274,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:P179"/>
+  <dimension ref="A2:P180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J166" sqref="J166"/>
+    <sheetView tabSelected="1" topLeftCell="A153" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K175" sqref="K175"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.28515625" customWidth="1"/>
-    <col min="11" max="11" width="35.42578125" customWidth="1"/>
-    <col min="12" max="12" width="26.7109375" customWidth="1"/>
-    <col min="16" max="16" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="53.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" customWidth="1"/>
+    <col min="11" max="11" width="35.44140625" customWidth="1"/>
+    <col min="12" max="12" width="26.6640625" customWidth="1"/>
+    <col min="16" max="16" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2307,7 +2318,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2316,11 +2327,11 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E996)</f>
-        <v>411.2</v>
+        <v>413.2</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>501.28000000000009</v>
+        <v>508.55000000000007</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
@@ -2329,34 +2340,34 @@
         <v>121.5</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="59" t="s">
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="75"/>
     </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="61"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="62"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
       <c r="J5" s="24"/>
       <c r="K5" s="75"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -2374,15 +2385,15 @@
       <c r="J6" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="69">
+      <c r="K6" s="59">
         <f>F7+F13+F20+F43+F45+F47+F46+J76+J133+J148+J164</f>
-        <v>91.320000000000007</v>
+        <v>98.59</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
@@ -2398,12 +2409,12 @@
       </c>
       <c r="G7" s="7"/>
       <c r="J7" s="77"/>
-      <c r="K7" s="69"/>
+      <c r="K7" s="59"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
@@ -2419,12 +2430,12 @@
       </c>
       <c r="G8" s="7"/>
       <c r="J8" s="78"/>
-      <c r="K8" s="69"/>
+      <c r="K8" s="59"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
@@ -2442,14 +2453,14 @@
       <c r="J9" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="69">
+      <c r="K9" s="59">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+J74+J131+J146+J162</f>
         <v>113.11000000000001</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>15</v>
       </c>
@@ -2465,9 +2476,9 @@
       </c>
       <c r="G10" s="7"/>
       <c r="J10" s="80"/>
-      <c r="K10" s="69"/>
-    </row>
-    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K10" s="59"/>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>16</v>
       </c>
@@ -2483,11 +2494,11 @@
       </c>
       <c r="G11" s="7"/>
       <c r="J11" s="81"/>
-      <c r="K11" s="69"/>
+      <c r="K11" s="59"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
@@ -2502,15 +2513,15 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="65" t="s">
+      <c r="J12" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="69">
+      <c r="K12" s="59">
         <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F48+F67+F68+J77+J134+J149+J165</f>
         <v>89.85</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>12</v>
       </c>
@@ -2525,10 +2536,10 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="69"/>
-    </row>
-    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J13" s="67"/>
+      <c r="K13" s="59"/>
+    </row>
+    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>13</v>
       </c>
@@ -2543,10 +2554,10 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="67"/>
-      <c r="K14" s="69"/>
-    </row>
-    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J14" s="68"/>
+      <c r="K14" s="59"/>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
@@ -2564,12 +2575,12 @@
       <c r="J15" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="69">
+      <c r="K15" s="59">
         <f>F10+F16+F39+F40+F49+F50+F51+J75+J132</f>
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
         <v>15</v>
       </c>
@@ -2585,9 +2596,9 @@
       </c>
       <c r="G16" s="7"/>
       <c r="J16" s="71"/>
-      <c r="K16" s="69"/>
-    </row>
-    <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K16" s="59"/>
+    </row>
+    <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>16</v>
       </c>
@@ -2603,9 +2614,9 @@
       </c>
       <c r="G17" s="7"/>
       <c r="J17" s="72"/>
-      <c r="K17" s="69"/>
-    </row>
-    <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K17" s="59"/>
+    </row>
+    <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>16</v>
       </c>
@@ -2625,12 +2636,12 @@
       <c r="J18" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="69">
+      <c r="K18" s="59">
         <f>F11+F23+F25+F27+F29+F31+F57+F58+F59+F60+F69+F70+J78+J135</f>
         <v>36.75</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>13</v>
       </c>
@@ -2649,9 +2660,9 @@
       </c>
       <c r="G19" s="7"/>
       <c r="J19" s="74"/>
-      <c r="K19" s="69"/>
-    </row>
-    <row r="20" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K19" s="59"/>
+    </row>
+    <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
@@ -2669,9 +2680,9 @@
       </c>
       <c r="G20" s="41"/>
       <c r="J20" s="74"/>
-      <c r="K20" s="69"/>
-    </row>
-    <row r="21" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K20" s="59"/>
+    </row>
+    <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
@@ -2689,7 +2700,7 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
@@ -2706,13 +2717,13 @@
         <v>5</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="J22" s="68" t="s">
+      <c r="J22" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="68"/>
-      <c r="L22" s="68"/>
-    </row>
-    <row r="23" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K22" s="69"/>
+      <c r="L22" s="69"/>
+    </row>
+    <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>16</v>
       </c>
@@ -2730,7 +2741,7 @@
       </c>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>13</v>
       </c>
@@ -2748,7 +2759,7 @@
       </c>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>16</v>
       </c>
@@ -2766,7 +2777,7 @@
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>13</v>
       </c>
@@ -2784,7 +2795,7 @@
       </c>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>16</v>
       </c>
@@ -2802,7 +2813,7 @@
       </c>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>13</v>
       </c>
@@ -2820,7 +2831,7 @@
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>16</v>
       </c>
@@ -2838,7 +2849,7 @@
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>13</v>
       </c>
@@ -2856,7 +2867,7 @@
       </c>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>16</v>
       </c>
@@ -2873,7 +2884,7 @@
       <c r="G31" s="7"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>14</v>
       </c>
@@ -2891,7 +2902,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
@@ -2907,7 +2918,7 @@
       </c>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>14</v>
       </c>
@@ -2925,7 +2936,7 @@
       </c>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>14</v>
       </c>
@@ -2943,7 +2954,7 @@
       </c>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
@@ -2961,7 +2972,7 @@
       </c>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>14</v>
       </c>
@@ -2979,7 +2990,7 @@
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>14</v>
       </c>
@@ -2997,7 +3008,7 @@
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>15</v>
       </c>
@@ -3015,7 +3026,7 @@
       </c>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>15</v>
       </c>
@@ -3033,25 +3044,25 @@
       </c>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B41" s="59" t="s">
+    <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B41" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="60"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="60"/>
-      <c r="G41" s="60"/>
-    </row>
-    <row r="42" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B42" s="61"/>
-      <c r="C42" s="62"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="62"/>
-      <c r="F42" s="62"/>
-      <c r="G42" s="62"/>
-    </row>
-    <row r="43" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="61"/>
+      <c r="F41" s="61"/>
+      <c r="G41" s="61"/>
+    </row>
+    <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B42" s="62"/>
+      <c r="C42" s="63"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="63"/>
+      <c r="F42" s="63"/>
+      <c r="G42" s="63"/>
+    </row>
+    <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>12</v>
       </c>
@@ -3069,7 +3080,7 @@
       </c>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>13</v>
       </c>
@@ -3087,7 +3098,7 @@
       </c>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>12</v>
       </c>
@@ -3105,7 +3116,7 @@
       </c>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>12</v>
       </c>
@@ -3123,7 +3134,7 @@
       </c>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>12</v>
       </c>
@@ -3141,7 +3152,7 @@
       </c>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>14</v>
       </c>
@@ -3159,7 +3170,7 @@
       </c>
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B49" s="9" t="s">
         <v>15</v>
       </c>
@@ -3186,7 +3197,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>15</v>
       </c>
@@ -3215,7 +3226,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
         <v>15</v>
       </c>
@@ -3244,7 +3255,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>9</v>
       </c>
@@ -3273,7 +3284,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>9</v>
       </c>
@@ -3302,7 +3313,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>9</v>
       </c>
@@ -3331,7 +3342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
         <v>13</v>
       </c>
@@ -3358,7 +3369,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="56" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
         <v>13</v>
       </c>
@@ -3376,7 +3387,7 @@
       </c>
       <c r="G56" s="11"/>
     </row>
-    <row r="57" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
         <v>16</v>
       </c>
@@ -3394,7 +3405,7 @@
       </c>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
         <v>16</v>
       </c>
@@ -3421,7 +3432,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>16</v>
       </c>
@@ -3450,7 +3461,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="60" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
         <v>16</v>
       </c>
@@ -3479,7 +3490,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B61" s="6" t="s">
         <v>13</v>
       </c>
@@ -3506,7 +3517,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
         <v>9</v>
       </c>
@@ -3535,7 +3546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
         <v>9</v>
       </c>
@@ -3564,7 +3575,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="64" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
         <v>9</v>
       </c>
@@ -3593,7 +3604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
         <v>9</v>
       </c>
@@ -3611,7 +3622,7 @@
       </c>
       <c r="G65" s="7"/>
     </row>
-    <row r="66" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="6" t="s">
         <v>13</v>
       </c>
@@ -3630,7 +3641,7 @@
       </c>
       <c r="G66" s="7"/>
     </row>
-    <row r="67" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="8" t="s">
         <v>14</v>
       </c>
@@ -3648,7 +3659,7 @@
       </c>
       <c r="G67" s="7"/>
     </row>
-    <row r="68" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="8" t="s">
         <v>14</v>
       </c>
@@ -3666,7 +3677,7 @@
       </c>
       <c r="G68" s="26"/>
     </row>
-    <row r="69" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="10" t="s">
         <v>16</v>
       </c>
@@ -3684,7 +3695,7 @@
       </c>
       <c r="G69" s="7"/>
     </row>
-    <row r="70" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="10" t="s">
         <v>16</v>
       </c>
@@ -3702,7 +3713,7 @@
       </c>
       <c r="G70" s="7"/>
     </row>
-    <row r="71" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
         <v>9</v>
       </c>
@@ -3720,15 +3731,15 @@
       </c>
       <c r="G71" s="7"/>
     </row>
-    <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="59" t="s">
+    <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="60"/>
-      <c r="D72" s="60"/>
-      <c r="E72" s="60"/>
-      <c r="F72" s="60"/>
-      <c r="G72" s="60"/>
+      <c r="C72" s="61"/>
+      <c r="D72" s="61"/>
+      <c r="E72" s="61"/>
+      <c r="F72" s="61"/>
+      <c r="G72" s="61"/>
       <c r="I72" s="33" t="s">
         <v>68</v>
       </c>
@@ -3739,13 +3750,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="61"/>
-      <c r="C73" s="62"/>
-      <c r="D73" s="62"/>
-      <c r="E73" s="62"/>
-      <c r="F73" s="62"/>
-      <c r="G73" s="62"/>
+    <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="62"/>
+      <c r="C73" s="63"/>
+      <c r="D73" s="63"/>
+      <c r="E73" s="63"/>
+      <c r="F73" s="63"/>
+      <c r="G73" s="63"/>
       <c r="I73" s="4" t="s">
         <v>9</v>
       </c>
@@ -3758,7 +3769,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="4" t="s">
         <v>9</v>
       </c>
@@ -3787,7 +3798,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
         <v>12</v>
       </c>
@@ -3816,7 +3827,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="76" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="9" t="s">
         <v>15</v>
       </c>
@@ -3843,7 +3854,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="9" t="s">
         <v>15</v>
       </c>
@@ -3872,7 +3883,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="9" t="s">
         <v>15</v>
       </c>
@@ -3901,7 +3912,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="79" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="10" t="s">
         <v>16</v>
       </c>
@@ -3917,7 +3928,7 @@
       </c>
       <c r="G79" s="11"/>
     </row>
-    <row r="80" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="6" t="s">
         <v>13</v>
       </c>
@@ -3933,7 +3944,7 @@
       </c>
       <c r="G80" s="49"/>
     </row>
-    <row r="81" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="10" t="s">
         <v>16</v>
       </c>
@@ -3947,7 +3958,7 @@
       <c r="F81" s="34"/>
       <c r="G81" s="34"/>
     </row>
-    <row r="82" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="10" t="s">
         <v>16</v>
       </c>
@@ -3965,7 +3976,7 @@
       </c>
       <c r="G82" s="11"/>
     </row>
-    <row r="83" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="4" t="s">
         <v>9</v>
       </c>
@@ -3983,7 +3994,7 @@
       </c>
       <c r="G83" s="7"/>
     </row>
-    <row r="84" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="8" t="s">
         <v>14</v>
       </c>
@@ -3997,7 +4008,7 @@
       <c r="F84" s="34"/>
       <c r="G84" s="34"/>
     </row>
-    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" s="8" t="s">
         <v>14</v>
       </c>
@@ -4011,7 +4022,7 @@
       <c r="F85" s="34"/>
       <c r="G85" s="34"/>
     </row>
-    <row r="86" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="8" t="s">
         <v>14</v>
       </c>
@@ -4025,7 +4036,7 @@
       <c r="F86" s="34"/>
       <c r="G86" s="34"/>
     </row>
-    <row r="87" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="36" t="s">
         <v>14</v>
       </c>
@@ -4043,7 +4054,7 @@
       </c>
       <c r="G87" s="37"/>
     </row>
-    <row r="88" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="9" t="s">
         <v>15</v>
       </c>
@@ -4061,7 +4072,7 @@
       </c>
       <c r="G88" s="49"/>
     </row>
-    <row r="89" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="5" t="s">
         <v>12</v>
       </c>
@@ -4079,7 +4090,7 @@
       </c>
       <c r="G89" s="7"/>
     </row>
-    <row r="90" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="5" t="s">
         <v>12</v>
       </c>
@@ -4097,7 +4108,7 @@
       </c>
       <c r="G90" s="7"/>
     </row>
-    <row r="91" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="6" t="s">
         <v>13</v>
       </c>
@@ -4115,7 +4126,7 @@
       </c>
       <c r="G91" s="11"/>
     </row>
-    <row r="92" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="s">
         <v>9</v>
       </c>
@@ -4133,7 +4144,7 @@
       </c>
       <c r="G92" s="11"/>
     </row>
-    <row r="93" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
         <v>9</v>
       </c>
@@ -4151,7 +4162,7 @@
       </c>
       <c r="G93" s="7"/>
     </row>
-    <row r="94" spans="2:7" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:7" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="4" t="s">
         <v>9</v>
       </c>
@@ -4169,7 +4180,7 @@
       </c>
       <c r="G94" s="7"/>
     </row>
-    <row r="95" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="4" t="s">
         <v>9</v>
       </c>
@@ -4187,7 +4198,7 @@
       </c>
       <c r="G95" s="7"/>
     </row>
-    <row r="96" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="40" t="s">
         <v>15</v>
       </c>
@@ -4205,7 +4216,7 @@
       </c>
       <c r="G96" s="7"/>
     </row>
-    <row r="97" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="10" t="s">
         <v>16</v>
       </c>
@@ -4223,7 +4234,7 @@
       </c>
       <c r="G97" s="7"/>
     </row>
-    <row r="98" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="37" t="s">
         <v>150</v>
       </c>
@@ -4237,7 +4248,7 @@
       <c r="F98" s="37"/>
       <c r="G98" s="11"/>
     </row>
-    <row r="99" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
         <v>12</v>
       </c>
@@ -4255,7 +4266,7 @@
       </c>
       <c r="G99" s="11"/>
     </row>
-    <row r="100" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="5" t="s">
         <v>12</v>
       </c>
@@ -4271,7 +4282,7 @@
       </c>
       <c r="G100" s="7"/>
     </row>
-    <row r="101" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="40" t="s">
         <v>15</v>
       </c>
@@ -4289,7 +4300,7 @@
       </c>
       <c r="G101" s="7"/>
     </row>
-    <row r="102" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="6" t="s">
         <v>13</v>
       </c>
@@ -4305,7 +4316,7 @@
       </c>
       <c r="G102" s="7"/>
     </row>
-    <row r="103" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="6" t="s">
         <v>13</v>
       </c>
@@ -4323,7 +4334,7 @@
       </c>
       <c r="G103" s="11"/>
     </row>
-    <row r="104" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="6" t="s">
         <v>13</v>
       </c>
@@ -4341,7 +4352,7 @@
       </c>
       <c r="G104" s="7"/>
     </row>
-    <row r="105" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="42" t="s">
         <v>9</v>
       </c>
@@ -4359,7 +4370,7 @@
       </c>
       <c r="G105" s="7"/>
     </row>
-    <row r="106" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="42" t="s">
         <v>9</v>
       </c>
@@ -4377,7 +4388,7 @@
       </c>
       <c r="G106" s="7"/>
     </row>
-    <row r="107" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="42" t="s">
         <v>9</v>
       </c>
@@ -4395,7 +4406,7 @@
       </c>
       <c r="G107" s="7"/>
     </row>
-    <row r="108" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="42" t="s">
         <v>9</v>
       </c>
@@ -4413,7 +4424,7 @@
       </c>
       <c r="G108" s="7"/>
     </row>
-    <row r="109" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="42" t="s">
         <v>9</v>
       </c>
@@ -4431,7 +4442,7 @@
       </c>
       <c r="G109" s="11"/>
     </row>
-    <row r="110" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="42" t="s">
         <v>9</v>
       </c>
@@ -4449,7 +4460,7 @@
       </c>
       <c r="G110" s="7"/>
     </row>
-    <row r="111" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="42" t="s">
         <v>9</v>
       </c>
@@ -4467,7 +4478,7 @@
       </c>
       <c r="G111" s="7"/>
     </row>
-    <row r="112" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="43" t="s">
         <v>14</v>
       </c>
@@ -4481,7 +4492,7 @@
       <c r="F112" s="34"/>
       <c r="G112" s="34"/>
     </row>
-    <row r="113" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="44" t="s">
         <v>14</v>
       </c>
@@ -4495,7 +4506,7 @@
       <c r="F113" s="34"/>
       <c r="G113" s="34"/>
     </row>
-    <row r="114" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="44" t="s">
         <v>14</v>
       </c>
@@ -4509,7 +4520,7 @@
       <c r="F114" s="34"/>
       <c r="G114" s="34"/>
     </row>
-    <row r="115" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="5" t="s">
         <v>12</v>
       </c>
@@ -4527,7 +4538,7 @@
       </c>
       <c r="G115" s="11"/>
     </row>
-    <row r="116" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="5" t="s">
         <v>12</v>
       </c>
@@ -4545,7 +4556,7 @@
       </c>
       <c r="G116" s="11"/>
     </row>
-    <row r="117" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="5" t="s">
         <v>12</v>
       </c>
@@ -4563,7 +4574,7 @@
       </c>
       <c r="G117" s="11"/>
     </row>
-    <row r="118" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="45" t="s">
         <v>13</v>
       </c>
@@ -4581,7 +4592,7 @@
       </c>
       <c r="G118" s="7"/>
     </row>
-    <row r="119" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="45" t="s">
         <v>13</v>
       </c>
@@ -4599,7 +4610,7 @@
       </c>
       <c r="G119" s="11"/>
     </row>
-    <row r="120" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="45" t="s">
         <v>13</v>
       </c>
@@ -4615,7 +4626,7 @@
       </c>
       <c r="G120" s="11"/>
     </row>
-    <row r="121" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="10" t="s">
         <v>16</v>
       </c>
@@ -4623,7 +4634,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="122" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B122" s="4" t="s">
         <v>9</v>
       </c>
@@ -4641,7 +4652,7 @@
       </c>
       <c r="G122" s="7"/>
     </row>
-    <row r="123" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" s="4" t="s">
         <v>9</v>
       </c>
@@ -4659,7 +4670,7 @@
       </c>
       <c r="G123" s="48"/>
     </row>
-    <row r="124" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="4" t="s">
         <v>9</v>
       </c>
@@ -4677,7 +4688,7 @@
       </c>
       <c r="G124" s="7"/>
     </row>
-    <row r="125" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" s="10" t="s">
         <v>16</v>
       </c>
@@ -4689,7 +4700,7 @@
       </c>
       <c r="G125" s="7"/>
     </row>
-    <row r="126" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" s="10" t="s">
         <v>16</v>
       </c>
@@ -4704,25 +4715,25 @@
       </c>
       <c r="G126" s="50"/>
     </row>
-    <row r="127" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B127" s="59" t="s">
+    <row r="127" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B127" s="60" t="s">
         <v>176</v>
       </c>
-      <c r="C127" s="60"/>
-      <c r="D127" s="60"/>
-      <c r="E127" s="60"/>
-      <c r="F127" s="60"/>
-      <c r="G127" s="60"/>
-    </row>
-    <row r="128" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B128" s="63"/>
-      <c r="C128" s="64"/>
-      <c r="D128" s="64"/>
-      <c r="E128" s="64"/>
-      <c r="F128" s="64"/>
-      <c r="G128" s="64"/>
-    </row>
-    <row r="129" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C127" s="61"/>
+      <c r="D127" s="61"/>
+      <c r="E127" s="61"/>
+      <c r="F127" s="61"/>
+      <c r="G127" s="61"/>
+    </row>
+    <row r="128" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B128" s="64"/>
+      <c r="C128" s="65"/>
+      <c r="D128" s="65"/>
+      <c r="E128" s="65"/>
+      <c r="F128" s="65"/>
+      <c r="G128" s="65"/>
+    </row>
+    <row r="129" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="51" t="s">
         <v>15</v>
       </c>
@@ -4747,7 +4758,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="130" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" s="51" t="s">
         <v>15</v>
       </c>
@@ -4774,7 +4785,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="131" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" s="52" t="s">
         <v>13</v>
       </c>
@@ -4801,7 +4812,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="52" t="s">
         <v>13</v>
       </c>
@@ -4828,7 +4839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="53" t="s">
         <v>16</v>
       </c>
@@ -4853,7 +4864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="134" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" s="55" t="s">
         <v>12</v>
       </c>
@@ -4869,7 +4880,7 @@
       <c r="F134" s="13">
         <v>17.399999999999999</v>
       </c>
-      <c r="G134" s="11"/>
+      <c r="G134" s="7"/>
       <c r="I134" s="8" t="s">
         <v>14</v>
       </c>
@@ -4882,7 +4893,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="56" t="s">
         <v>14</v>
       </c>
@@ -4905,7 +4916,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B136" s="56" t="s">
         <v>14</v>
       </c>
@@ -4919,7 +4930,7 @@
       </c>
       <c r="G136" s="11"/>
     </row>
-    <row r="137" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="54" t="s">
         <v>9</v>
       </c>
@@ -4937,7 +4948,7 @@
       </c>
       <c r="G137" s="11"/>
     </row>
-    <row r="138" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="54" t="s">
         <v>9</v>
       </c>
@@ -4955,7 +4966,7 @@
       </c>
       <c r="G138" s="7"/>
     </row>
-    <row r="139" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" s="54" t="s">
         <v>9</v>
       </c>
@@ -4973,7 +4984,7 @@
       </c>
       <c r="G139" s="7"/>
     </row>
-    <row r="140" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B140" s="54" t="s">
         <v>9</v>
       </c>
@@ -4991,7 +5002,7 @@
       </c>
       <c r="G140" s="7"/>
     </row>
-    <row r="141" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B141" s="53" t="s">
         <v>16</v>
       </c>
@@ -5007,25 +5018,25 @@
       </c>
       <c r="G141" s="7"/>
     </row>
-    <row r="142" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B142" s="59" t="s">
+    <row r="142" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B142" s="60" t="s">
         <v>187</v>
       </c>
-      <c r="C142" s="60"/>
-      <c r="D142" s="60"/>
-      <c r="E142" s="60"/>
-      <c r="F142" s="60"/>
-      <c r="G142" s="60"/>
-    </row>
-    <row r="143" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B143" s="63"/>
-      <c r="C143" s="64"/>
-      <c r="D143" s="64"/>
-      <c r="E143" s="64"/>
-      <c r="F143" s="64"/>
-      <c r="G143" s="64"/>
-    </row>
-    <row r="144" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C142" s="61"/>
+      <c r="D142" s="61"/>
+      <c r="E142" s="61"/>
+      <c r="F142" s="61"/>
+      <c r="G142" s="61"/>
+    </row>
+    <row r="143" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B143" s="64"/>
+      <c r="C143" s="65"/>
+      <c r="D143" s="65"/>
+      <c r="E143" s="65"/>
+      <c r="F143" s="65"/>
+      <c r="G143" s="65"/>
+    </row>
+    <row r="144" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="55" t="s">
         <v>12</v>
       </c>
@@ -5052,7 +5063,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="145" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="55" t="s">
         <v>12</v>
       </c>
@@ -5081,7 +5092,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="146" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B146" s="53" t="s">
         <v>16</v>
       </c>
@@ -5104,7 +5115,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B147" s="55" t="s">
         <v>12</v>
       </c>
@@ -5118,12 +5129,12 @@
       <c r="F147" s="13">
         <v>6.34</v>
       </c>
-      <c r="G147" s="11"/>
+      <c r="G147" s="50"/>
       <c r="I147" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" s="52" t="s">
         <v>13</v>
       </c>
@@ -5152,7 +5163,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="149" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B149" s="52" t="s">
         <v>13</v>
       </c>
@@ -5177,7 +5188,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="150" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B150" s="52" t="s">
         <v>13</v>
       </c>
@@ -5194,7 +5205,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="151" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B151" s="52" t="s">
         <v>13</v>
       </c>
@@ -5212,7 +5223,7 @@
       </c>
       <c r="G151" s="11"/>
     </row>
-    <row r="152" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B152" s="54" t="s">
         <v>9</v>
       </c>
@@ -5230,7 +5241,7 @@
       </c>
       <c r="G152" s="11"/>
     </row>
-    <row r="153" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B153" s="54" t="s">
         <v>9</v>
       </c>
@@ -5248,7 +5259,7 @@
       </c>
       <c r="G153" s="7"/>
     </row>
-    <row r="154" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B154" s="54" t="s">
         <v>9</v>
       </c>
@@ -5264,7 +5275,7 @@
       <c r="F154" s="13"/>
       <c r="G154" s="26"/>
     </row>
-    <row r="155" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B155" s="51" t="s">
         <v>15</v>
       </c>
@@ -5280,7 +5291,7 @@
       </c>
       <c r="G155" s="11"/>
     </row>
-    <row r="156" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156" s="51" t="s">
         <v>15</v>
       </c>
@@ -5294,7 +5305,7 @@
       <c r="F156" s="13"/>
       <c r="G156" s="11"/>
     </row>
-    <row r="157" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" s="56" t="s">
         <v>14</v>
       </c>
@@ -5310,7 +5321,7 @@
       </c>
       <c r="G157" s="11"/>
     </row>
-    <row r="158" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158" s="56" t="s">
         <v>14</v>
       </c>
@@ -5326,23 +5337,23 @@
       </c>
       <c r="G158" s="7"/>
     </row>
-    <row r="159" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B159" s="59" t="s">
+    <row r="159" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B159" s="60" t="s">
         <v>201</v>
       </c>
-      <c r="C159" s="60"/>
-      <c r="D159" s="60"/>
-      <c r="E159" s="60"/>
-      <c r="F159" s="60"/>
-      <c r="G159" s="60"/>
-    </row>
-    <row r="160" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B160" s="63"/>
-      <c r="C160" s="64"/>
-      <c r="D160" s="64"/>
-      <c r="E160" s="64"/>
-      <c r="F160" s="64"/>
-      <c r="G160" s="64"/>
+      <c r="C159" s="61"/>
+      <c r="D159" s="61"/>
+      <c r="E159" s="61"/>
+      <c r="F159" s="61"/>
+      <c r="G159" s="61"/>
+    </row>
+    <row r="160" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B160" s="64"/>
+      <c r="C160" s="65"/>
+      <c r="D160" s="65"/>
+      <c r="E160" s="65"/>
+      <c r="F160" s="65"/>
+      <c r="G160" s="65"/>
       <c r="I160" s="58" t="s">
         <v>188</v>
       </c>
@@ -5353,7 +5364,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="161" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B161" s="56" t="s">
         <v>14</v>
       </c>
@@ -5372,7 +5383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="162" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B162" s="56" t="s">
         <v>14</v>
       </c>
@@ -5395,7 +5406,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="163" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163" s="56" t="s">
         <v>14</v>
       </c>
@@ -5410,7 +5421,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B164" s="56" t="s">
         <v>14</v>
       </c>
@@ -5425,15 +5436,15 @@
         <v>12</v>
       </c>
       <c r="J164">
-        <f>F165+F166+F179</f>
-        <v>10.48</v>
+        <f>F165+F166+F179+F180</f>
+        <v>17.75</v>
       </c>
       <c r="K164">
         <f>E165+E166+E179</f>
         <v>16</v>
       </c>
     </row>
-    <row r="165" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B165" s="55" t="s">
         <v>12</v>
       </c>
@@ -5443,7 +5454,7 @@
       <c r="D165" s="13"/>
       <c r="E165" s="13"/>
       <c r="F165" s="13"/>
-      <c r="G165" s="1"/>
+      <c r="G165" s="50"/>
       <c r="I165" s="8" t="s">
         <v>14</v>
       </c>
@@ -5456,7 +5467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B166" s="55" t="s">
         <v>12</v>
       </c>
@@ -5468,14 +5479,14 @@
         <v>15</v>
       </c>
       <c r="F166" s="13">
-        <v>6.48</v>
-      </c>
-      <c r="G166" s="1"/>
+        <v>13.5</v>
+      </c>
+      <c r="G166" s="7"/>
       <c r="I166" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="167" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B167" s="54" t="s">
         <v>9</v>
       </c>
@@ -5487,7 +5498,7 @@
       <c r="F167" s="13"/>
       <c r="G167" s="1"/>
     </row>
-    <row r="168" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B168" s="54" t="s">
         <v>9</v>
       </c>
@@ -5499,7 +5510,7 @@
       <c r="F168" s="13"/>
       <c r="G168" s="1"/>
     </row>
-    <row r="169" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B169" s="54" t="s">
         <v>9</v>
       </c>
@@ -5517,7 +5528,7 @@
       </c>
       <c r="G169" s="7"/>
     </row>
-    <row r="170" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" s="54" t="s">
         <v>9</v>
       </c>
@@ -5535,7 +5546,7 @@
       </c>
       <c r="G170" s="7"/>
     </row>
-    <row r="171" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B171" s="52" t="s">
         <v>13</v>
       </c>
@@ -5553,7 +5564,7 @@
       </c>
       <c r="G171" s="11"/>
     </row>
-    <row r="172" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172" s="52" t="s">
         <v>13</v>
       </c>
@@ -5571,7 +5582,7 @@
       </c>
       <c r="G172" s="7"/>
     </row>
-    <row r="173" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173" s="52" t="s">
         <v>13</v>
       </c>
@@ -5589,7 +5600,7 @@
       </c>
       <c r="G173" s="11"/>
     </row>
-    <row r="174" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B174" s="52" t="s">
         <v>13</v>
       </c>
@@ -5605,7 +5616,7 @@
       </c>
       <c r="G174" s="50"/>
     </row>
-    <row r="175" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175" s="53" t="s">
         <v>16</v>
       </c>
@@ -5617,7 +5628,7 @@
       <c r="F175" s="13"/>
       <c r="G175" s="1"/>
     </row>
-    <row r="176" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176" s="53" t="s">
         <v>16</v>
       </c>
@@ -5627,7 +5638,7 @@
       <c r="F176" s="13"/>
       <c r="G176" s="1"/>
     </row>
-    <row r="177" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177" s="51" t="s">
         <v>15</v>
       </c>
@@ -5639,7 +5650,7 @@
       <c r="F177" s="13"/>
       <c r="G177" s="1"/>
     </row>
-    <row r="178" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B178" s="51" t="s">
         <v>15</v>
       </c>
@@ -5651,7 +5662,7 @@
       <c r="F178" s="13"/>
       <c r="G178" s="1"/>
     </row>
-    <row r="179" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B179" s="55" t="s">
         <v>12</v>
       </c>
@@ -5667,8 +5678,26 @@
       </c>
       <c r="G179" s="7"/>
     </row>
+    <row r="180" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B180" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="C180" s="82" t="s">
+        <v>219</v>
+      </c>
+      <c r="D180" s="13"/>
+      <c r="E180" s="13">
+        <v>2</v>
+      </c>
+      <c r="F180" s="82">
+        <v>0.25</v>
+      </c>
+      <c r="G180" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="J9:J11"/>
     <mergeCell ref="K9:K11"/>
     <mergeCell ref="B72:G73"/>
     <mergeCell ref="B41:G42"/>
@@ -5685,8 +5714,6 @@
     <mergeCell ref="J18:J20"/>
     <mergeCell ref="K3:K5"/>
     <mergeCell ref="J6:J8"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="J9:J11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5706,17 +5733,17 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>91</v>
       </c>
@@ -5746,7 +5773,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -5775,7 +5802,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -5798,7 +5825,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -5821,7 +5848,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -5836,7 +5863,7 @@
       <c r="F5" s="13"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -5855,7 +5882,7 @@
       </c>
       <c r="G6" s="27"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -5878,7 +5905,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -5893,7 +5920,7 @@
       <c r="F8" s="13"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -5916,7 +5943,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>9</v>
       </c>
@@ -5931,7 +5958,7 @@
       <c r="F10" s="13"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>10</v>
       </c>
@@ -5946,7 +5973,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>11</v>
       </c>
@@ -5963,7 +5990,7 @@
       <c r="F12" s="13"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>12</v>
       </c>
@@ -5978,7 +6005,7 @@
       <c r="F13" s="13"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -5995,7 +6022,7 @@
       <c r="F14" s="13"/>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>14</v>
       </c>
@@ -6010,7 +6037,7 @@
       <c r="F15" s="13"/>
       <c r="G15" s="15"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>15</v>
       </c>
@@ -6025,7 +6052,7 @@
       <c r="F16" s="13"/>
       <c r="G16" s="15"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>16</v>
       </c>
@@ -6040,7 +6067,7 @@
       <c r="F17" s="13"/>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -6063,7 +6090,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -6086,7 +6113,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -6100,7 +6127,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -6121,7 +6148,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -6136,7 +6163,7 @@
       <c r="F22" s="13"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -6151,7 +6178,7 @@
       <c r="F23" s="13"/>
       <c r="G23" s="15"/>
     </row>
-    <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -6172,7 +6199,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -6187,7 +6214,7 @@
       <c r="F25" s="13"/>
       <c r="G25" s="15"/>
     </row>
-    <row r="26" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -6210,7 +6237,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -6225,7 +6252,7 @@
       <c r="F27" s="13"/>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -6248,7 +6275,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -6263,7 +6290,7 @@
       <c r="F29" s="13"/>
       <c r="G29" s="15"/>
     </row>
-    <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -6280,7 +6307,7 @@
       <c r="F30" s="13"/>
       <c r="G30" s="15"/>
     </row>
-    <row r="31" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -6303,7 +6330,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>31</v>
       </c>
@@ -6324,7 +6351,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>32</v>
       </c>
@@ -6345,7 +6372,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>33</v>
       </c>
@@ -6368,7 +6395,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>34</v>
       </c>
@@ -6385,7 +6412,7 @@
       <c r="F35" s="13"/>
       <c r="G35" s="15"/>
     </row>
-    <row r="36" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>35</v>
       </c>
@@ -6400,7 +6427,7 @@
       <c r="F36" s="13"/>
       <c r="G36" s="15"/>
     </row>
-    <row r="37" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>36</v>
       </c>
@@ -6423,7 +6450,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>37</v>
       </c>
@@ -6440,7 +6467,7 @@
       <c r="F38" s="13"/>
       <c r="G38" s="15"/>
     </row>
-    <row r="39" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>38</v>
       </c>
@@ -6455,7 +6482,7 @@
       <c r="F39" s="13"/>
       <c r="G39" s="15"/>
     </row>
-    <row r="40" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>39</v>
       </c>
@@ -6476,7 +6503,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>40</v>
       </c>
@@ -6499,7 +6526,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>41</v>
       </c>
@@ -6522,7 +6549,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>42</v>
       </c>
@@ -6545,7 +6572,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <v>43</v>
       </c>
@@ -6568,7 +6595,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>44</v>
       </c>
@@ -6589,7 +6616,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>45</v>
       </c>
@@ -6606,7 +6633,7 @@
       <c r="F46" s="13"/>
       <c r="G46" s="15"/>
     </row>
-    <row r="47" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>46</v>
       </c>
@@ -6627,7 +6654,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <v>47</v>
       </c>
@@ -6650,7 +6677,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="38">
         <v>48</v>
       </c>
@@ -6676,6 +6703,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6884,38 +6928,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6938,9 +6954,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Blackjack con reglas y recompensas
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 6ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 6ª Version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\DaniPC\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745939AE-14B8-4E19-A545-A79B3E6007B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58B7541-DA7D-47C0-9598-05BD04725727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1186,7 +1186,17 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1246,16 +1256,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2276,8 +2276,8 @@
   </sheetPr>
   <dimension ref="A2:P180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K175" sqref="K175"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I172" sqref="I172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2331,38 +2331,38 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>508.55000000000007</v>
+        <v>509.05000000000007</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="75">
+      <c r="K3" s="79">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73+J130+J145</f>
         <v>121.5</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="75"/>
+      <c r="K4" s="79"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="62"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="75"/>
+      <c r="K5" s="79"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
@@ -2382,12 +2382,12 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="76" t="s">
+      <c r="J6" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="59">
+      <c r="K6" s="60">
         <f>F7+F13+F20+F43+F45+F47+F46+J76+J133+J148+J164</f>
-        <v>98.59</v>
+        <v>99.09</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -2408,8 +2408,8 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="59"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="60"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="P7" s="2"/>
@@ -2429,8 +2429,8 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="59"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="60"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="O8" s="2"/>
@@ -2450,10 +2450,10 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="79" t="s">
+      <c r="J9" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="59">
+      <c r="K9" s="60">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+J74+J131+J146+J162</f>
         <v>113.11000000000001</v>
       </c>
@@ -2475,8 +2475,8 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="80"/>
-      <c r="K10" s="59"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="60"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
@@ -2493,8 +2493,8 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="59"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="60"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
@@ -2513,10 +2513,10 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="66" t="s">
+      <c r="J12" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="59">
+      <c r="K12" s="60">
         <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F48+F67+F68+J77+J134+J149+J165</f>
         <v>89.85</v>
       </c>
@@ -2536,8 +2536,8 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="59"/>
+      <c r="J13" s="71"/>
+      <c r="K13" s="60"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -2554,8 +2554,8 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="59"/>
+      <c r="J14" s="72"/>
+      <c r="K14" s="60"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -2572,10 +2572,10 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="70" t="s">
+      <c r="J15" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="59">
+      <c r="K15" s="60">
         <f>F10+F16+F39+F40+F49+F50+F51+J75+J132</f>
         <v>42</v>
       </c>
@@ -2595,8 +2595,8 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="71"/>
-      <c r="K16" s="59"/>
+      <c r="J16" s="75"/>
+      <c r="K16" s="60"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
@@ -2613,8 +2613,8 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="72"/>
-      <c r="K17" s="59"/>
+      <c r="J17" s="76"/>
+      <c r="K17" s="60"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
@@ -2633,10 +2633,10 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="73" t="s">
+      <c r="J18" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="59">
+      <c r="K18" s="60">
         <f>F11+F23+F25+F27+F29+F31+F57+F58+F59+F60+F69+F70+J78+J135</f>
         <v>36.75</v>
       </c>
@@ -2659,8 +2659,8 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="74"/>
-      <c r="K19" s="59"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="60"/>
     </row>
     <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
@@ -2679,8 +2679,8 @@
         <v>20</v>
       </c>
       <c r="G20" s="41"/>
-      <c r="J20" s="74"/>
-      <c r="K20" s="59"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="60"/>
     </row>
     <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
@@ -2717,11 +2717,11 @@
         <v>5</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="J22" s="69" t="s">
+      <c r="J22" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="69"/>
-      <c r="L22" s="69"/>
+      <c r="K22" s="73"/>
+      <c r="L22" s="73"/>
     </row>
     <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
@@ -3045,22 +3045,22 @@
       <c r="G40" s="7"/>
     </row>
     <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B41" s="60" t="s">
+      <c r="B41" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="61"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
+      <c r="C41" s="65"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="65"/>
+      <c r="F41" s="65"/>
+      <c r="G41" s="65"/>
     </row>
     <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B42" s="62"/>
-      <c r="C42" s="63"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="63"/>
-      <c r="F42" s="63"/>
-      <c r="G42" s="63"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="67"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="67"/>
+      <c r="F42" s="67"/>
+      <c r="G42" s="67"/>
     </row>
     <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
@@ -3732,14 +3732,14 @@
       <c r="G71" s="7"/>
     </row>
     <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="60" t="s">
+      <c r="B72" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="61"/>
-      <c r="D72" s="61"/>
-      <c r="E72" s="61"/>
-      <c r="F72" s="61"/>
-      <c r="G72" s="61"/>
+      <c r="C72" s="65"/>
+      <c r="D72" s="65"/>
+      <c r="E72" s="65"/>
+      <c r="F72" s="65"/>
+      <c r="G72" s="65"/>
       <c r="I72" s="33" t="s">
         <v>68</v>
       </c>
@@ -3751,12 +3751,12 @@
       </c>
     </row>
     <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="62"/>
-      <c r="C73" s="63"/>
-      <c r="D73" s="63"/>
-      <c r="E73" s="63"/>
-      <c r="F73" s="63"/>
-      <c r="G73" s="63"/>
+      <c r="B73" s="66"/>
+      <c r="C73" s="67"/>
+      <c r="D73" s="67"/>
+      <c r="E73" s="67"/>
+      <c r="F73" s="67"/>
+      <c r="G73" s="67"/>
       <c r="I73" s="4" t="s">
         <v>9</v>
       </c>
@@ -4716,22 +4716,22 @@
       <c r="G126" s="50"/>
     </row>
     <row r="127" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="60" t="s">
+      <c r="B127" s="64" t="s">
         <v>176</v>
       </c>
-      <c r="C127" s="61"/>
-      <c r="D127" s="61"/>
-      <c r="E127" s="61"/>
-      <c r="F127" s="61"/>
-      <c r="G127" s="61"/>
+      <c r="C127" s="65"/>
+      <c r="D127" s="65"/>
+      <c r="E127" s="65"/>
+      <c r="F127" s="65"/>
+      <c r="G127" s="65"/>
     </row>
     <row r="128" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="64"/>
-      <c r="C128" s="65"/>
-      <c r="D128" s="65"/>
-      <c r="E128" s="65"/>
-      <c r="F128" s="65"/>
-      <c r="G128" s="65"/>
+      <c r="B128" s="68"/>
+      <c r="C128" s="69"/>
+      <c r="D128" s="69"/>
+      <c r="E128" s="69"/>
+      <c r="F128" s="69"/>
+      <c r="G128" s="69"/>
     </row>
     <row r="129" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="51" t="s">
@@ -5019,22 +5019,22 @@
       <c r="G141" s="7"/>
     </row>
     <row r="142" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="60" t="s">
+      <c r="B142" s="64" t="s">
         <v>187</v>
       </c>
-      <c r="C142" s="61"/>
-      <c r="D142" s="61"/>
-      <c r="E142" s="61"/>
-      <c r="F142" s="61"/>
-      <c r="G142" s="61"/>
+      <c r="C142" s="65"/>
+      <c r="D142" s="65"/>
+      <c r="E142" s="65"/>
+      <c r="F142" s="65"/>
+      <c r="G142" s="65"/>
     </row>
     <row r="143" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="64"/>
-      <c r="C143" s="65"/>
-      <c r="D143" s="65"/>
-      <c r="E143" s="65"/>
-      <c r="F143" s="65"/>
-      <c r="G143" s="65"/>
+      <c r="B143" s="68"/>
+      <c r="C143" s="69"/>
+      <c r="D143" s="69"/>
+      <c r="E143" s="69"/>
+      <c r="F143" s="69"/>
+      <c r="G143" s="69"/>
     </row>
     <row r="144" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="55" t="s">
@@ -5338,22 +5338,22 @@
       <c r="G158" s="7"/>
     </row>
     <row r="159" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="60" t="s">
+      <c r="B159" s="64" t="s">
         <v>201</v>
       </c>
-      <c r="C159" s="61"/>
-      <c r="D159" s="61"/>
-      <c r="E159" s="61"/>
-      <c r="F159" s="61"/>
-      <c r="G159" s="61"/>
+      <c r="C159" s="65"/>
+      <c r="D159" s="65"/>
+      <c r="E159" s="65"/>
+      <c r="F159" s="65"/>
+      <c r="G159" s="65"/>
     </row>
     <row r="160" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B160" s="64"/>
-      <c r="C160" s="65"/>
-      <c r="D160" s="65"/>
-      <c r="E160" s="65"/>
-      <c r="F160" s="65"/>
-      <c r="G160" s="65"/>
+      <c r="B160" s="68"/>
+      <c r="C160" s="69"/>
+      <c r="D160" s="69"/>
+      <c r="E160" s="69"/>
+      <c r="F160" s="69"/>
+      <c r="G160" s="69"/>
       <c r="I160" s="58" t="s">
         <v>188</v>
       </c>
@@ -5437,7 +5437,7 @@
       </c>
       <c r="J164">
         <f>F165+F166+F179+F180</f>
-        <v>17.75</v>
+        <v>18.25</v>
       </c>
       <c r="K164">
         <f>E165+E166+E179</f>
@@ -5682,25 +5682,20 @@
       <c r="B180" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="C180" s="82" t="s">
+      <c r="C180" s="59" t="s">
         <v>219</v>
       </c>
       <c r="D180" s="13"/>
       <c r="E180" s="13">
         <v>2</v>
       </c>
-      <c r="F180" s="82">
-        <v>0.25</v>
+      <c r="F180" s="59">
+        <v>0.75</v>
       </c>
       <c r="G180" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="B72:G73"/>
-    <mergeCell ref="B41:G42"/>
     <mergeCell ref="B159:G160"/>
     <mergeCell ref="B4:G5"/>
     <mergeCell ref="J12:J14"/>
@@ -5714,6 +5709,11 @@
     <mergeCell ref="J18:J20"/>
     <mergeCell ref="K3:K5"/>
     <mergeCell ref="J6:J8"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="B72:G73"/>
+    <mergeCell ref="B41:G42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6703,23 +6703,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6928,10 +6911,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6954,20 +6965,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>